<commit_message>
Cambios con vales cerrados
Hicieron falta cosas del backend
</commit_message>
<xml_diff>
--- a/documents/ReporteVale.xlsx
+++ b/documents/ReporteVale.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David Duarte Garcia\OneDrive - Universidad Técnica Nacional\Escritorio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{301C120F-E069-44AD-BE91-0475B5B13018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4874BF8-2615-4E24-854E-9234BF605845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{C8E842AF-28D0-4143-9950-C0C2C392F242}"/>
   </bookViews>
@@ -241,7 +241,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\-mm\-yy"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="MS Sans Serif"/>
@@ -379,6 +379,10 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="MS Sans Serif"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1130,10 +1134,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1374,6 +1374,48 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1406,14 +1448,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="14" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
@@ -1481,48 +1515,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1577,6 +1569,51 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
     </xf>
@@ -1603,51 +1640,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
     </xf>
@@ -1686,6 +1678,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous" vertical="top"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2023,8 +2027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{505F8341-330E-4B75-B029-434DF2C2CA09}">
   <dimension ref="B1:AT113"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="AA47" sqref="AA47"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2034,10 +2038,10 @@
     <col min="3" max="3" width="4.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="4" style="1" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" style="1" customWidth="1"/>
     <col min="7" max="7" width="18.42578125" style="1" customWidth="1"/>
     <col min="8" max="8" width="10.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="2" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" style="1" customWidth="1"/>
     <col min="10" max="10" width="9.5703125" style="1" customWidth="1"/>
     <col min="11" max="11" width="16.85546875" style="1" customWidth="1"/>
     <col min="12" max="12" width="3.28515625" style="1" hidden="1" customWidth="1"/>
@@ -3763,926 +3767,926 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="168" t="s">
+      <c r="B1" s="165" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="168"/>
-      <c r="D1" s="168"/>
-      <c r="E1" s="168"/>
-      <c r="F1" s="168"/>
-      <c r="G1" s="168"/>
-      <c r="H1" s="168"/>
-      <c r="I1" s="168"/>
-      <c r="J1" s="168"/>
-      <c r="K1" s="168"/>
-      <c r="N1" s="169" t="s">
+      <c r="C1" s="165"/>
+      <c r="D1" s="165"/>
+      <c r="E1" s="165"/>
+      <c r="F1" s="165"/>
+      <c r="G1" s="165"/>
+      <c r="H1" s="165"/>
+      <c r="I1" s="165"/>
+      <c r="J1" s="165"/>
+      <c r="K1" s="165"/>
+      <c r="N1" s="166" t="s">
         <v>33</v>
       </c>
-      <c r="O1" s="169"/>
-      <c r="P1" s="169"/>
-      <c r="Q1" s="169"/>
-      <c r="R1" s="169"/>
-      <c r="S1" s="169"/>
-      <c r="T1" s="169"/>
-      <c r="U1" s="169"/>
-      <c r="V1" s="169"/>
-      <c r="W1" s="169"/>
-      <c r="X1" s="169"/>
-      <c r="Y1" s="169"/>
-      <c r="Z1" s="169"/>
-      <c r="AA1" s="169"/>
-      <c r="AB1" s="63"/>
+      <c r="O1" s="166"/>
+      <c r="P1" s="166"/>
+      <c r="Q1" s="166"/>
+      <c r="R1" s="166"/>
+      <c r="S1" s="166"/>
+      <c r="T1" s="166"/>
+      <c r="U1" s="166"/>
+      <c r="V1" s="166"/>
+      <c r="W1" s="166"/>
+      <c r="X1" s="166"/>
+      <c r="Y1" s="166"/>
+      <c r="Z1" s="166"/>
+      <c r="AA1" s="166"/>
+      <c r="AB1" s="62"/>
     </row>
     <row r="2" spans="2:28" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="170" t="s">
+      <c r="B2" s="167" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="170"/>
-      <c r="D2" s="170"/>
-      <c r="E2" s="170"/>
-      <c r="F2" s="170"/>
-      <c r="G2" s="170"/>
-      <c r="H2" s="170"/>
-      <c r="I2" s="170"/>
-      <c r="J2" s="170"/>
+      <c r="C2" s="167"/>
+      <c r="D2" s="167"/>
+      <c r="E2" s="167"/>
+      <c r="F2" s="167"/>
+      <c r="G2" s="167"/>
+      <c r="H2" s="167"/>
+      <c r="I2" s="167"/>
+      <c r="J2" s="167"/>
       <c r="N2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AB2" s="63"/>
+      <c r="AB2" s="62"/>
     </row>
     <row r="3" spans="2:28" ht="12.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="171" t="s">
+      <c r="B3" s="168" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="171"/>
-      <c r="D3" s="171"/>
-      <c r="E3" s="171"/>
-      <c r="F3" s="171"/>
-      <c r="G3" s="171"/>
-      <c r="H3" s="171"/>
-      <c r="I3" s="171"/>
-      <c r="J3" s="171"/>
-      <c r="N3" s="172" t="s">
+      <c r="C3" s="168"/>
+      <c r="D3" s="168"/>
+      <c r="E3" s="168"/>
+      <c r="F3" s="168"/>
+      <c r="G3" s="168"/>
+      <c r="H3" s="168"/>
+      <c r="I3" s="168"/>
+      <c r="J3" s="168"/>
+      <c r="N3" s="169" t="s">
         <v>34</v>
       </c>
-      <c r="O3" s="173"/>
-      <c r="P3" s="174"/>
-      <c r="Q3" s="174"/>
-      <c r="R3" s="174"/>
-      <c r="S3" s="174"/>
-      <c r="T3" s="174"/>
-      <c r="U3" s="174"/>
-      <c r="V3" s="175"/>
-      <c r="W3" s="176" t="s">
+      <c r="O3" s="170"/>
+      <c r="P3" s="171"/>
+      <c r="Q3" s="171"/>
+      <c r="R3" s="171"/>
+      <c r="S3" s="171"/>
+      <c r="T3" s="171"/>
+      <c r="U3" s="171"/>
+      <c r="V3" s="172"/>
+      <c r="W3" s="173" t="s">
         <v>35</v>
       </c>
-      <c r="X3" s="174"/>
-      <c r="Y3" s="174"/>
-      <c r="Z3" s="174"/>
-      <c r="AA3" s="177"/>
-      <c r="AB3" s="63"/>
+      <c r="X3" s="171"/>
+      <c r="Y3" s="171"/>
+      <c r="Z3" s="171"/>
+      <c r="AA3" s="174"/>
+      <c r="AB3" s="62"/>
     </row>
     <row r="4" spans="2:28" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="170" t="s">
+      <c r="B4" s="167" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="170"/>
-      <c r="D4" s="170"/>
-      <c r="E4" s="170"/>
-      <c r="F4" s="170"/>
-      <c r="G4" s="170"/>
-      <c r="H4" s="170"/>
-      <c r="I4" s="170"/>
-      <c r="J4" s="170"/>
-      <c r="N4" s="54" t="s">
+      <c r="C4" s="167"/>
+      <c r="D4" s="167"/>
+      <c r="E4" s="167"/>
+      <c r="F4" s="167"/>
+      <c r="G4" s="167"/>
+      <c r="H4" s="167"/>
+      <c r="I4" s="167"/>
+      <c r="J4" s="167"/>
+      <c r="N4" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="O4" s="55"/>
-      <c r="P4" s="178" t="s">
+      <c r="O4" s="54"/>
+      <c r="P4" s="175" t="s">
         <v>36</v>
       </c>
-      <c r="Q4" s="178"/>
-      <c r="R4" s="178"/>
-      <c r="S4" s="178"/>
-      <c r="T4" s="178"/>
-      <c r="U4" s="178"/>
-      <c r="V4" s="179"/>
-      <c r="W4" s="56" t="s">
+      <c r="Q4" s="175"/>
+      <c r="R4" s="175"/>
+      <c r="S4" s="175"/>
+      <c r="T4" s="175"/>
+      <c r="U4" s="175"/>
+      <c r="V4" s="176"/>
+      <c r="W4" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="X4" s="57"/>
-      <c r="Y4" s="180" t="s">
+      <c r="X4" s="56"/>
+      <c r="Y4" s="177" t="s">
         <v>37</v>
       </c>
-      <c r="Z4" s="178"/>
-      <c r="AA4" s="58"/>
-      <c r="AB4" s="63"/>
+      <c r="Z4" s="175"/>
+      <c r="AA4" s="57"/>
+      <c r="AB4" s="62"/>
     </row>
     <row r="5" spans="2:28" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="159" t="s">
+      <c r="B5" s="148" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="160"/>
-      <c r="D5" s="160"/>
-      <c r="E5" s="160"/>
-      <c r="F5" s="160"/>
-      <c r="G5" s="160"/>
-      <c r="H5" s="160"/>
-      <c r="I5" s="161"/>
-      <c r="J5" s="48" t="s">
+      <c r="C5" s="149"/>
+      <c r="D5" s="149"/>
+      <c r="E5" s="149"/>
+      <c r="F5" s="149"/>
+      <c r="G5" s="149"/>
+      <c r="H5" s="149"/>
+      <c r="I5" s="150"/>
+      <c r="J5" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="K5" s="47"/>
-      <c r="N5" s="59" t="s">
+      <c r="K5" s="46"/>
+      <c r="N5" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="O5" s="60" t="s">
+      <c r="O5" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="P5" s="134" t="s">
+      <c r="P5" s="131" t="s">
         <v>39</v>
       </c>
-      <c r="Q5" s="162"/>
-      <c r="R5" s="162"/>
-      <c r="S5" s="162"/>
-      <c r="T5" s="162"/>
-      <c r="U5" s="162"/>
-      <c r="V5" s="135"/>
-      <c r="W5" s="134" t="s">
+      <c r="Q5" s="151"/>
+      <c r="R5" s="151"/>
+      <c r="S5" s="151"/>
+      <c r="T5" s="151"/>
+      <c r="U5" s="151"/>
+      <c r="V5" s="132"/>
+      <c r="W5" s="131" t="s">
         <v>40</v>
       </c>
-      <c r="X5" s="162"/>
-      <c r="Y5" s="162"/>
-      <c r="Z5" s="162"/>
-      <c r="AA5" s="163"/>
-      <c r="AB5" s="63"/>
+      <c r="X5" s="151"/>
+      <c r="Y5" s="151"/>
+      <c r="Z5" s="151"/>
+      <c r="AA5" s="152"/>
+      <c r="AB5" s="62"/>
     </row>
     <row r="6" spans="2:28" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="46" t="s">
+      <c r="B6" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="45"/>
-      <c r="I6" s="45"/>
-      <c r="J6" s="45"/>
-      <c r="K6" s="44"/>
-      <c r="N6" s="83" t="s">
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="44"/>
+      <c r="K6" s="43"/>
+      <c r="N6" s="82" t="s">
         <v>41</v>
       </c>
-      <c r="O6" s="70"/>
-      <c r="P6" s="72" t="s">
+      <c r="O6" s="69"/>
+      <c r="P6" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="Q6" s="74"/>
-      <c r="R6" s="74"/>
-      <c r="S6" s="76" t="s">
+      <c r="Q6" s="73"/>
+      <c r="R6" s="73"/>
+      <c r="S6" s="75" t="s">
         <v>43</v>
       </c>
-      <c r="T6" s="74"/>
-      <c r="U6" s="78"/>
-      <c r="V6" s="80"/>
-      <c r="W6" s="81"/>
-      <c r="X6" s="81"/>
-      <c r="Y6" s="81"/>
-      <c r="Z6" s="81"/>
-      <c r="AA6" s="82"/>
-      <c r="AB6" s="63"/>
+      <c r="T6" s="73"/>
+      <c r="U6" s="77"/>
+      <c r="V6" s="79"/>
+      <c r="W6" s="80"/>
+      <c r="X6" s="80"/>
+      <c r="Y6" s="80"/>
+      <c r="Z6" s="80"/>
+      <c r="AA6" s="81"/>
+      <c r="AB6" s="62"/>
     </row>
     <row r="7" spans="2:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="147" t="s">
+      <c r="B7" s="157" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="148"/>
-      <c r="D7" s="149" t="s">
+      <c r="C7" s="158"/>
+      <c r="D7" s="159" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="150"/>
-      <c r="F7" s="153"/>
-      <c r="G7" s="153"/>
-      <c r="H7" s="153"/>
-      <c r="I7" s="153"/>
-      <c r="J7" s="153"/>
-      <c r="K7" s="43" t="s">
+      <c r="E7" s="160"/>
+      <c r="F7" s="163"/>
+      <c r="G7" s="163"/>
+      <c r="H7" s="163"/>
+      <c r="I7" s="163"/>
+      <c r="J7" s="163"/>
+      <c r="K7" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="N7" s="84"/>
-      <c r="O7" s="71"/>
-      <c r="P7" s="73"/>
-      <c r="Q7" s="75"/>
-      <c r="R7" s="75"/>
-      <c r="S7" s="77"/>
-      <c r="T7" s="75"/>
-      <c r="U7" s="79"/>
-      <c r="V7" s="80"/>
-      <c r="W7" s="81"/>
-      <c r="X7" s="81"/>
-      <c r="Y7" s="81"/>
-      <c r="Z7" s="81"/>
-      <c r="AA7" s="82"/>
-      <c r="AB7" s="63"/>
+      <c r="N7" s="83"/>
+      <c r="O7" s="70"/>
+      <c r="P7" s="72"/>
+      <c r="Q7" s="74"/>
+      <c r="R7" s="74"/>
+      <c r="S7" s="76"/>
+      <c r="T7" s="74"/>
+      <c r="U7" s="78"/>
+      <c r="V7" s="79"/>
+      <c r="W7" s="80"/>
+      <c r="X7" s="80"/>
+      <c r="Y7" s="80"/>
+      <c r="Z7" s="80"/>
+      <c r="AA7" s="81"/>
+      <c r="AB7" s="62"/>
     </row>
     <row r="8" spans="2:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="155"/>
-      <c r="C8" s="156"/>
-      <c r="D8" s="151"/>
-      <c r="E8" s="152"/>
-      <c r="F8" s="154"/>
-      <c r="G8" s="154"/>
-      <c r="H8" s="154"/>
-      <c r="I8" s="154"/>
-      <c r="J8" s="154"/>
-      <c r="K8" s="42"/>
-      <c r="N8" s="83" t="s">
+      <c r="B8" s="144"/>
+      <c r="C8" s="145"/>
+      <c r="D8" s="161"/>
+      <c r="E8" s="162"/>
+      <c r="F8" s="164"/>
+      <c r="G8" s="164"/>
+      <c r="H8" s="164"/>
+      <c r="I8" s="164"/>
+      <c r="J8" s="164"/>
+      <c r="K8" s="41"/>
+      <c r="N8" s="82" t="s">
         <v>44</v>
       </c>
-      <c r="O8" s="70"/>
-      <c r="P8" s="72" t="s">
+      <c r="O8" s="69"/>
+      <c r="P8" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="Q8" s="74"/>
-      <c r="R8" s="74"/>
-      <c r="S8" s="76" t="s">
+      <c r="Q8" s="73"/>
+      <c r="R8" s="73"/>
+      <c r="S8" s="75" t="s">
         <v>43</v>
       </c>
-      <c r="T8" s="74"/>
-      <c r="U8" s="78"/>
-      <c r="V8" s="80"/>
-      <c r="W8" s="81"/>
-      <c r="X8" s="81"/>
-      <c r="Y8" s="81"/>
-      <c r="Z8" s="81"/>
-      <c r="AA8" s="82"/>
-      <c r="AB8" s="63"/>
+      <c r="T8" s="73"/>
+      <c r="U8" s="77"/>
+      <c r="V8" s="79"/>
+      <c r="W8" s="80"/>
+      <c r="X8" s="80"/>
+      <c r="Y8" s="80"/>
+      <c r="Z8" s="80"/>
+      <c r="AA8" s="81"/>
+      <c r="AB8" s="62"/>
     </row>
     <row r="9" spans="2:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="41" t="s">
+      <c r="B9" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="164"/>
-      <c r="D9" s="164"/>
-      <c r="E9" s="164"/>
-      <c r="F9" s="164"/>
-      <c r="G9" s="164"/>
-      <c r="H9" s="164"/>
-      <c r="I9" s="164"/>
-      <c r="J9" s="164"/>
-      <c r="K9" s="165"/>
-      <c r="N9" s="84"/>
-      <c r="O9" s="71"/>
-      <c r="P9" s="73"/>
-      <c r="Q9" s="75"/>
-      <c r="R9" s="75"/>
-      <c r="S9" s="77"/>
-      <c r="T9" s="75"/>
-      <c r="U9" s="79"/>
-      <c r="V9" s="80"/>
-      <c r="W9" s="81"/>
-      <c r="X9" s="81"/>
-      <c r="Y9" s="81"/>
-      <c r="Z9" s="81"/>
-      <c r="AA9" s="82"/>
-      <c r="AB9" s="63"/>
+      <c r="C9" s="153"/>
+      <c r="D9" s="153"/>
+      <c r="E9" s="153"/>
+      <c r="F9" s="153"/>
+      <c r="G9" s="153"/>
+      <c r="H9" s="153"/>
+      <c r="I9" s="153"/>
+      <c r="J9" s="153"/>
+      <c r="K9" s="154"/>
+      <c r="N9" s="83"/>
+      <c r="O9" s="70"/>
+      <c r="P9" s="72"/>
+      <c r="Q9" s="74"/>
+      <c r="R9" s="74"/>
+      <c r="S9" s="76"/>
+      <c r="T9" s="74"/>
+      <c r="U9" s="78"/>
+      <c r="V9" s="79"/>
+      <c r="W9" s="80"/>
+      <c r="X9" s="80"/>
+      <c r="Y9" s="80"/>
+      <c r="Z9" s="80"/>
+      <c r="AA9" s="81"/>
+      <c r="AB9" s="62"/>
     </row>
     <row r="10" spans="2:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="40"/>
-      <c r="C10" s="145"/>
-      <c r="D10" s="145"/>
-      <c r="E10" s="145"/>
-      <c r="F10" s="145"/>
-      <c r="G10" s="145"/>
-      <c r="H10" s="145"/>
-      <c r="I10" s="145"/>
-      <c r="J10" s="145"/>
-      <c r="K10" s="166"/>
-      <c r="N10" s="83" t="s">
+      <c r="B10" s="39"/>
+      <c r="C10" s="142"/>
+      <c r="D10" s="142"/>
+      <c r="E10" s="142"/>
+      <c r="F10" s="142"/>
+      <c r="G10" s="142"/>
+      <c r="H10" s="142"/>
+      <c r="I10" s="142"/>
+      <c r="J10" s="142"/>
+      <c r="K10" s="155"/>
+      <c r="N10" s="82" t="s">
         <v>45</v>
       </c>
-      <c r="O10" s="70"/>
-      <c r="P10" s="72" t="s">
+      <c r="O10" s="69"/>
+      <c r="P10" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="Q10" s="74"/>
-      <c r="R10" s="74"/>
-      <c r="S10" s="74" t="s">
+      <c r="Q10" s="73"/>
+      <c r="R10" s="73"/>
+      <c r="S10" s="73" t="s">
         <v>43</v>
       </c>
-      <c r="T10" s="74"/>
-      <c r="U10" s="78"/>
-      <c r="V10" s="80"/>
-      <c r="W10" s="81"/>
-      <c r="X10" s="81"/>
-      <c r="Y10" s="81"/>
-      <c r="Z10" s="81"/>
-      <c r="AA10" s="82"/>
-      <c r="AB10" s="63"/>
+      <c r="T10" s="73"/>
+      <c r="U10" s="77"/>
+      <c r="V10" s="79"/>
+      <c r="W10" s="80"/>
+      <c r="X10" s="80"/>
+      <c r="Y10" s="80"/>
+      <c r="Z10" s="80"/>
+      <c r="AA10" s="81"/>
+      <c r="AB10" s="62"/>
     </row>
     <row r="11" spans="2:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="39"/>
-      <c r="C11" s="167"/>
-      <c r="D11" s="167"/>
-      <c r="E11" s="167"/>
-      <c r="F11" s="167"/>
-      <c r="G11" s="167"/>
-      <c r="H11" s="167"/>
-      <c r="I11" s="145"/>
-      <c r="J11" s="145"/>
-      <c r="K11" s="166"/>
-      <c r="N11" s="84"/>
-      <c r="O11" s="71"/>
-      <c r="P11" s="73"/>
-      <c r="Q11" s="75"/>
-      <c r="R11" s="75"/>
-      <c r="S11" s="75"/>
-      <c r="T11" s="75"/>
-      <c r="U11" s="79"/>
-      <c r="V11" s="80"/>
-      <c r="W11" s="81"/>
-      <c r="X11" s="81"/>
-      <c r="Y11" s="81"/>
-      <c r="Z11" s="81"/>
-      <c r="AA11" s="82"/>
-      <c r="AB11" s="63"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="156"/>
+      <c r="D11" s="156"/>
+      <c r="E11" s="156"/>
+      <c r="F11" s="156"/>
+      <c r="G11" s="156"/>
+      <c r="H11" s="156"/>
+      <c r="I11" s="142"/>
+      <c r="J11" s="142"/>
+      <c r="K11" s="155"/>
+      <c r="N11" s="83"/>
+      <c r="O11" s="70"/>
+      <c r="P11" s="72"/>
+      <c r="Q11" s="74"/>
+      <c r="R11" s="74"/>
+      <c r="S11" s="74"/>
+      <c r="T11" s="74"/>
+      <c r="U11" s="78"/>
+      <c r="V11" s="79"/>
+      <c r="W11" s="80"/>
+      <c r="X11" s="80"/>
+      <c r="Y11" s="80"/>
+      <c r="Z11" s="80"/>
+      <c r="AA11" s="81"/>
+      <c r="AB11" s="62"/>
     </row>
     <row r="12" spans="2:28" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="157" t="s">
+      <c r="B12" s="146" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="158"/>
-      <c r="D12" s="158"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="37" t="s">
+      <c r="C12" s="147"/>
+      <c r="D12" s="147"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="I12" s="141"/>
-      <c r="J12" s="142"/>
-      <c r="K12" s="143"/>
-      <c r="N12" s="83" t="s">
+      <c r="I12" s="138"/>
+      <c r="J12" s="139"/>
+      <c r="K12" s="140"/>
+      <c r="N12" s="82" t="s">
         <v>46</v>
       </c>
-      <c r="O12" s="70"/>
-      <c r="P12" s="72" t="s">
+      <c r="O12" s="69"/>
+      <c r="P12" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="Q12" s="74"/>
-      <c r="R12" s="74"/>
-      <c r="S12" s="76" t="s">
+      <c r="Q12" s="73"/>
+      <c r="R12" s="73"/>
+      <c r="S12" s="75" t="s">
         <v>43</v>
       </c>
-      <c r="T12" s="74"/>
-      <c r="U12" s="78"/>
-      <c r="V12" s="80"/>
-      <c r="W12" s="81"/>
-      <c r="X12" s="81"/>
-      <c r="Y12" s="81"/>
-      <c r="Z12" s="81"/>
-      <c r="AA12" s="82"/>
-      <c r="AB12" s="63"/>
+      <c r="T12" s="73"/>
+      <c r="U12" s="77"/>
+      <c r="V12" s="79"/>
+      <c r="W12" s="80"/>
+      <c r="X12" s="80"/>
+      <c r="Y12" s="80"/>
+      <c r="Z12" s="80"/>
+      <c r="AA12" s="81"/>
+      <c r="AB12" s="62"/>
     </row>
     <row r="13" spans="2:28" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="144"/>
-      <c r="C13" s="145"/>
-      <c r="D13" s="145"/>
-      <c r="E13" s="145"/>
-      <c r="F13" s="145"/>
-      <c r="G13" s="145"/>
-      <c r="H13" s="146"/>
-      <c r="I13" s="141"/>
-      <c r="J13" s="142"/>
-      <c r="K13" s="143"/>
-      <c r="N13" s="84"/>
-      <c r="O13" s="71"/>
-      <c r="P13" s="73"/>
-      <c r="Q13" s="75"/>
-      <c r="R13" s="75"/>
-      <c r="S13" s="77"/>
-      <c r="T13" s="75"/>
-      <c r="U13" s="79"/>
-      <c r="V13" s="80"/>
-      <c r="W13" s="81"/>
-      <c r="X13" s="81"/>
-      <c r="Y13" s="81"/>
-      <c r="Z13" s="81"/>
-      <c r="AA13" s="82"/>
-      <c r="AB13" s="63"/>
+      <c r="B13" s="141"/>
+      <c r="C13" s="142"/>
+      <c r="D13" s="142"/>
+      <c r="E13" s="142"/>
+      <c r="F13" s="142"/>
+      <c r="G13" s="142"/>
+      <c r="H13" s="143"/>
+      <c r="I13" s="138"/>
+      <c r="J13" s="139"/>
+      <c r="K13" s="140"/>
+      <c r="N13" s="83"/>
+      <c r="O13" s="70"/>
+      <c r="P13" s="72"/>
+      <c r="Q13" s="74"/>
+      <c r="R13" s="74"/>
+      <c r="S13" s="76"/>
+      <c r="T13" s="74"/>
+      <c r="U13" s="78"/>
+      <c r="V13" s="79"/>
+      <c r="W13" s="80"/>
+      <c r="X13" s="80"/>
+      <c r="Y13" s="80"/>
+      <c r="Z13" s="80"/>
+      <c r="AA13" s="81"/>
+      <c r="AB13" s="62"/>
     </row>
     <row r="14" spans="2:28" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="50"/>
-      <c r="C14" s="51"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="51"/>
-      <c r="F14" s="51"/>
-      <c r="G14" s="51"/>
-      <c r="H14" s="51"/>
-      <c r="I14" s="141"/>
-      <c r="J14" s="142"/>
-      <c r="K14" s="143"/>
-      <c r="N14" s="68" t="s">
+      <c r="B14" s="49"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="50"/>
+      <c r="E14" s="50"/>
+      <c r="F14" s="50"/>
+      <c r="G14" s="50"/>
+      <c r="H14" s="50"/>
+      <c r="I14" s="138"/>
+      <c r="J14" s="139"/>
+      <c r="K14" s="140"/>
+      <c r="N14" s="67" t="s">
         <v>47</v>
       </c>
-      <c r="O14" s="70"/>
-      <c r="P14" s="72" t="s">
+      <c r="O14" s="69"/>
+      <c r="P14" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="Q14" s="74"/>
-      <c r="R14" s="74"/>
-      <c r="S14" s="76" t="s">
+      <c r="Q14" s="73"/>
+      <c r="R14" s="73"/>
+      <c r="S14" s="75" t="s">
         <v>43</v>
       </c>
-      <c r="T14" s="74"/>
-      <c r="U14" s="78"/>
-      <c r="V14" s="80"/>
-      <c r="W14" s="81"/>
-      <c r="X14" s="81"/>
-      <c r="Y14" s="81"/>
-      <c r="Z14" s="81"/>
-      <c r="AA14" s="82"/>
-      <c r="AB14" s="63"/>
+      <c r="T14" s="73"/>
+      <c r="U14" s="77"/>
+      <c r="V14" s="79"/>
+      <c r="W14" s="80"/>
+      <c r="X14" s="80"/>
+      <c r="Y14" s="80"/>
+      <c r="Z14" s="80"/>
+      <c r="AA14" s="81"/>
+      <c r="AB14" s="62"/>
     </row>
     <row r="15" spans="2:28" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="50"/>
-      <c r="C15" s="51"/>
-      <c r="D15" s="51"/>
-      <c r="E15" s="51"/>
-      <c r="F15" s="51"/>
-      <c r="G15" s="51"/>
-      <c r="H15" s="51"/>
-      <c r="I15" s="141"/>
-      <c r="J15" s="142"/>
-      <c r="K15" s="143"/>
-      <c r="N15" s="69"/>
-      <c r="O15" s="71"/>
-      <c r="P15" s="73"/>
-      <c r="Q15" s="75"/>
-      <c r="R15" s="75"/>
-      <c r="S15" s="77"/>
-      <c r="T15" s="75"/>
-      <c r="U15" s="79"/>
-      <c r="V15" s="80"/>
-      <c r="W15" s="81"/>
-      <c r="X15" s="81"/>
-      <c r="Y15" s="81"/>
-      <c r="Z15" s="81"/>
-      <c r="AA15" s="82"/>
-      <c r="AB15" s="63"/>
+      <c r="B15" s="49"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="50"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="50"/>
+      <c r="H15" s="50"/>
+      <c r="I15" s="138"/>
+      <c r="J15" s="139"/>
+      <c r="K15" s="140"/>
+      <c r="N15" s="68"/>
+      <c r="O15" s="70"/>
+      <c r="P15" s="72"/>
+      <c r="Q15" s="74"/>
+      <c r="R15" s="74"/>
+      <c r="S15" s="76"/>
+      <c r="T15" s="74"/>
+      <c r="U15" s="78"/>
+      <c r="V15" s="79"/>
+      <c r="W15" s="80"/>
+      <c r="X15" s="80"/>
+      <c r="Y15" s="80"/>
+      <c r="Z15" s="80"/>
+      <c r="AA15" s="81"/>
+      <c r="AB15" s="62"/>
     </row>
     <row r="16" spans="2:28" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="50"/>
-      <c r="C16" s="51"/>
-      <c r="D16" s="51"/>
-      <c r="E16" s="51"/>
-      <c r="F16" s="51"/>
-      <c r="G16" s="51"/>
-      <c r="H16" s="52"/>
-      <c r="I16" s="141"/>
-      <c r="J16" s="142"/>
-      <c r="K16" s="143"/>
-      <c r="N16" s="83" t="s">
+      <c r="B16" s="49"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="50"/>
+      <c r="E16" s="50"/>
+      <c r="F16" s="50"/>
+      <c r="G16" s="50"/>
+      <c r="H16" s="51"/>
+      <c r="I16" s="138"/>
+      <c r="J16" s="139"/>
+      <c r="K16" s="140"/>
+      <c r="N16" s="82" t="s">
         <v>48</v>
       </c>
-      <c r="O16" s="70"/>
-      <c r="P16" s="72" t="s">
+      <c r="O16" s="69"/>
+      <c r="P16" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="Q16" s="74"/>
-      <c r="R16" s="74"/>
-      <c r="S16" s="76" t="s">
+      <c r="Q16" s="73"/>
+      <c r="R16" s="73"/>
+      <c r="S16" s="75" t="s">
         <v>43</v>
       </c>
-      <c r="T16" s="74"/>
-      <c r="U16" s="78"/>
-      <c r="V16" s="80"/>
-      <c r="W16" s="81"/>
-      <c r="X16" s="81"/>
-      <c r="Y16" s="81"/>
-      <c r="Z16" s="81"/>
-      <c r="AA16" s="82"/>
-      <c r="AB16" s="63"/>
+      <c r="T16" s="73"/>
+      <c r="U16" s="77"/>
+      <c r="V16" s="79"/>
+      <c r="W16" s="80"/>
+      <c r="X16" s="80"/>
+      <c r="Y16" s="80"/>
+      <c r="Z16" s="80"/>
+      <c r="AA16" s="81"/>
+      <c r="AB16" s="62"/>
     </row>
     <row r="17" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="131" t="s">
+      <c r="B17" s="128" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="132"/>
-      <c r="D17" s="132"/>
-      <c r="E17" s="132"/>
-      <c r="F17" s="133"/>
-      <c r="G17" s="136"/>
-      <c r="H17" s="137"/>
-      <c r="I17" s="137"/>
-      <c r="J17" s="137"/>
-      <c r="K17" s="138"/>
-      <c r="N17" s="84"/>
-      <c r="O17" s="71"/>
-      <c r="P17" s="73"/>
-      <c r="Q17" s="75"/>
-      <c r="R17" s="75"/>
-      <c r="S17" s="77"/>
-      <c r="T17" s="75"/>
-      <c r="U17" s="79"/>
-      <c r="V17" s="80"/>
-      <c r="W17" s="81"/>
-      <c r="X17" s="81"/>
-      <c r="Y17" s="81"/>
-      <c r="Z17" s="81"/>
-      <c r="AA17" s="82"/>
-      <c r="AB17" s="63"/>
+      <c r="C17" s="129"/>
+      <c r="D17" s="129"/>
+      <c r="E17" s="129"/>
+      <c r="F17" s="130"/>
+      <c r="G17" s="133"/>
+      <c r="H17" s="134"/>
+      <c r="I17" s="134"/>
+      <c r="J17" s="134"/>
+      <c r="K17" s="135"/>
+      <c r="N17" s="83"/>
+      <c r="O17" s="70"/>
+      <c r="P17" s="72"/>
+      <c r="Q17" s="74"/>
+      <c r="R17" s="74"/>
+      <c r="S17" s="76"/>
+      <c r="T17" s="74"/>
+      <c r="U17" s="78"/>
+      <c r="V17" s="79"/>
+      <c r="W17" s="80"/>
+      <c r="X17" s="80"/>
+      <c r="Y17" s="80"/>
+      <c r="Z17" s="80"/>
+      <c r="AA17" s="81"/>
+      <c r="AB17" s="62"/>
     </row>
     <row r="18" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="36"/>
-      <c r="C18" s="134" t="s">
+      <c r="B18" s="35"/>
+      <c r="C18" s="131" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="135"/>
-      <c r="E18" s="134" t="s">
+      <c r="D18" s="132"/>
+      <c r="E18" s="131" t="s">
         <v>20</v>
       </c>
-      <c r="F18" s="135"/>
-      <c r="G18" s="49" t="s">
+      <c r="F18" s="132"/>
+      <c r="G18" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="H18" s="139"/>
-      <c r="I18" s="139"/>
-      <c r="J18" s="139"/>
-      <c r="K18" s="140"/>
-      <c r="N18" s="111" t="s">
+      <c r="H18" s="136"/>
+      <c r="I18" s="136"/>
+      <c r="J18" s="136"/>
+      <c r="K18" s="137"/>
+      <c r="N18" s="122" t="s">
         <v>49</v>
       </c>
-      <c r="O18" s="114"/>
-      <c r="P18" s="117" t="s">
+      <c r="O18" s="125"/>
+      <c r="P18" s="84" t="s">
         <v>42</v>
       </c>
-      <c r="Q18" s="117"/>
-      <c r="R18" s="117"/>
-      <c r="S18" s="120" t="s">
+      <c r="Q18" s="84"/>
+      <c r="R18" s="84"/>
+      <c r="S18" s="87" t="s">
         <v>43</v>
       </c>
-      <c r="T18" s="74"/>
-      <c r="U18" s="74"/>
-      <c r="V18" s="80"/>
-      <c r="W18" s="81"/>
-      <c r="X18" s="81"/>
-      <c r="Y18" s="81"/>
-      <c r="Z18" s="81"/>
-      <c r="AA18" s="82"/>
-      <c r="AB18" s="63"/>
+      <c r="T18" s="73"/>
+      <c r="U18" s="73"/>
+      <c r="V18" s="79"/>
+      <c r="W18" s="80"/>
+      <c r="X18" s="80"/>
+      <c r="Y18" s="80"/>
+      <c r="Z18" s="80"/>
+      <c r="AA18" s="81"/>
+      <c r="AB18" s="62"/>
     </row>
     <row r="19" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="33" t="s">
+      <c r="B19" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="104"/>
-      <c r="D19" s="105"/>
-      <c r="E19" s="106"/>
-      <c r="F19" s="107"/>
-      <c r="G19" s="35" t="s">
+      <c r="C19" s="115"/>
+      <c r="D19" s="116"/>
+      <c r="E19" s="117"/>
+      <c r="F19" s="118"/>
+      <c r="G19" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="H19" s="34"/>
-      <c r="I19" s="34"/>
-      <c r="J19" s="108"/>
-      <c r="K19" s="109"/>
-      <c r="N19" s="112"/>
-      <c r="O19" s="115"/>
-      <c r="P19" s="118"/>
-      <c r="Q19" s="118"/>
-      <c r="R19" s="118"/>
-      <c r="S19" s="121"/>
-      <c r="T19" s="123"/>
-      <c r="U19" s="123"/>
-      <c r="V19" s="124"/>
-      <c r="W19" s="74"/>
-      <c r="X19" s="74"/>
-      <c r="Y19" s="74"/>
-      <c r="Z19" s="74"/>
-      <c r="AA19" s="125"/>
-      <c r="AB19" s="63"/>
+      <c r="H19" s="33"/>
+      <c r="I19" s="33"/>
+      <c r="J19" s="119"/>
+      <c r="K19" s="120"/>
+      <c r="N19" s="123"/>
+      <c r="O19" s="126"/>
+      <c r="P19" s="85"/>
+      <c r="Q19" s="85"/>
+      <c r="R19" s="85"/>
+      <c r="S19" s="88"/>
+      <c r="T19" s="90"/>
+      <c r="U19" s="90"/>
+      <c r="V19" s="91"/>
+      <c r="W19" s="73"/>
+      <c r="X19" s="73"/>
+      <c r="Y19" s="73"/>
+      <c r="Z19" s="73"/>
+      <c r="AA19" s="92"/>
+      <c r="AB19" s="62"/>
     </row>
     <row r="20" spans="2:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="33" t="s">
+      <c r="B20" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="101"/>
-      <c r="D20" s="110"/>
-      <c r="E20" s="101"/>
-      <c r="F20" s="102"/>
-      <c r="G20" s="32"/>
-      <c r="H20" s="31"/>
-      <c r="I20" s="31"/>
-      <c r="J20" s="75" t="s">
+      <c r="C20" s="112"/>
+      <c r="D20" s="121"/>
+      <c r="E20" s="112"/>
+      <c r="F20" s="113"/>
+      <c r="G20" s="31"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="74" t="s">
         <v>16</v>
       </c>
-      <c r="K20" s="103"/>
-      <c r="N20" s="113"/>
-      <c r="O20" s="116"/>
-      <c r="P20" s="119"/>
-      <c r="Q20" s="119"/>
-      <c r="R20" s="119"/>
-      <c r="S20" s="122"/>
-      <c r="T20" s="75"/>
-      <c r="U20" s="75"/>
-      <c r="V20" s="126"/>
-      <c r="W20" s="75"/>
-      <c r="X20" s="75"/>
-      <c r="Y20" s="75"/>
-      <c r="Z20" s="75"/>
-      <c r="AA20" s="127"/>
-      <c r="AB20" s="63"/>
+      <c r="K20" s="114"/>
+      <c r="N20" s="124"/>
+      <c r="O20" s="127"/>
+      <c r="P20" s="86"/>
+      <c r="Q20" s="86"/>
+      <c r="R20" s="86"/>
+      <c r="S20" s="89"/>
+      <c r="T20" s="74"/>
+      <c r="U20" s="74"/>
+      <c r="V20" s="93"/>
+      <c r="W20" s="74"/>
+      <c r="X20" s="74"/>
+      <c r="Y20" s="74"/>
+      <c r="Z20" s="74"/>
+      <c r="AA20" s="94"/>
+      <c r="AB20" s="62"/>
     </row>
     <row r="21" spans="2:28" ht="1.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="21">
+      <c r="B21" s="20">
         <v>2</v>
       </c>
-      <c r="C21" s="30" t="s">
+      <c r="C21" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="30"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="30"/>
-      <c r="G21" s="29"/>
-      <c r="H21" s="29"/>
-      <c r="I21" s="29"/>
-      <c r="J21" s="29"/>
-      <c r="K21" s="28"/>
-      <c r="N21" s="128" t="s">
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="28"/>
+      <c r="I21" s="28"/>
+      <c r="J21" s="28"/>
+      <c r="K21" s="27"/>
+      <c r="N21" s="95" t="s">
         <v>50</v>
       </c>
-      <c r="O21" s="129"/>
-      <c r="P21" s="129"/>
-      <c r="Q21" s="129"/>
-      <c r="R21" s="129"/>
-      <c r="S21" s="129"/>
-      <c r="T21" s="129"/>
-      <c r="U21" s="129"/>
-      <c r="V21" s="129"/>
-      <c r="W21" s="129"/>
-      <c r="X21" s="129"/>
-      <c r="Y21" s="129"/>
-      <c r="Z21" s="129"/>
-      <c r="AA21" s="130"/>
-      <c r="AB21" s="63"/>
+      <c r="O21" s="96"/>
+      <c r="P21" s="96"/>
+      <c r="Q21" s="96"/>
+      <c r="R21" s="96"/>
+      <c r="S21" s="96"/>
+      <c r="T21" s="96"/>
+      <c r="U21" s="96"/>
+      <c r="V21" s="96"/>
+      <c r="W21" s="96"/>
+      <c r="X21" s="96"/>
+      <c r="Y21" s="96"/>
+      <c r="Z21" s="96"/>
+      <c r="AA21" s="97"/>
+      <c r="AB21" s="62"/>
     </row>
     <row r="22" spans="2:28" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="85" t="s">
+      <c r="B22" s="98" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="86"/>
-      <c r="D22" s="86"/>
-      <c r="E22" s="86"/>
-      <c r="F22" s="86"/>
-      <c r="G22" s="86"/>
-      <c r="H22" s="86"/>
-      <c r="I22" s="86"/>
-      <c r="J22" s="86"/>
-      <c r="K22" s="93"/>
-      <c r="N22" s="67" t="s">
+      <c r="C22" s="99"/>
+      <c r="D22" s="99"/>
+      <c r="E22" s="99"/>
+      <c r="F22" s="99"/>
+      <c r="G22" s="99"/>
+      <c r="H22" s="99"/>
+      <c r="I22" s="99"/>
+      <c r="J22" s="99"/>
+      <c r="K22" s="106"/>
+      <c r="N22" s="66" t="s">
         <v>51</v>
       </c>
-      <c r="O22" s="67"/>
-      <c r="P22" s="67"/>
-      <c r="Q22" s="67"/>
-      <c r="R22" s="67"/>
-      <c r="S22" s="67"/>
-      <c r="T22" s="67"/>
-      <c r="U22" s="67"/>
-      <c r="V22" s="67"/>
-      <c r="W22" s="67"/>
-      <c r="X22" s="67"/>
-      <c r="Y22" s="67"/>
-      <c r="Z22" s="67"/>
-      <c r="AA22" s="67"/>
-      <c r="AB22" s="63"/>
+      <c r="O22" s="66"/>
+      <c r="P22" s="66"/>
+      <c r="Q22" s="66"/>
+      <c r="R22" s="66"/>
+      <c r="S22" s="66"/>
+      <c r="T22" s="66"/>
+      <c r="U22" s="66"/>
+      <c r="V22" s="66"/>
+      <c r="W22" s="66"/>
+      <c r="X22" s="66"/>
+      <c r="Y22" s="66"/>
+      <c r="Z22" s="66"/>
+      <c r="AA22" s="66"/>
+      <c r="AB22" s="62"/>
     </row>
     <row r="23" spans="2:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="85" t="s">
+      <c r="B23" s="98" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="86"/>
-      <c r="D23" s="86"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="27" t="s">
+      <c r="C23" s="99"/>
+      <c r="D23" s="99"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="25"/>
+      <c r="H23" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="I23" s="26"/>
-      <c r="J23" s="26"/>
-      <c r="K23" s="25"/>
-      <c r="N23" s="66" t="s">
+      <c r="I23" s="25"/>
+      <c r="J23" s="25"/>
+      <c r="K23" s="24"/>
+      <c r="N23" s="65" t="s">
         <v>52</v>
       </c>
-      <c r="O23" s="66"/>
-      <c r="P23" s="66"/>
-      <c r="Q23" s="66"/>
-      <c r="R23" s="66"/>
-      <c r="S23" s="66"/>
-      <c r="T23" s="66"/>
-      <c r="U23" s="66"/>
-      <c r="V23" s="66"/>
-      <c r="W23" s="66"/>
-      <c r="X23" s="66"/>
-      <c r="Y23" s="66"/>
-      <c r="Z23" s="66"/>
-      <c r="AA23" s="66"/>
-      <c r="AB23" s="63"/>
+      <c r="O23" s="65"/>
+      <c r="P23" s="65"/>
+      <c r="Q23" s="65"/>
+      <c r="R23" s="65"/>
+      <c r="S23" s="65"/>
+      <c r="T23" s="65"/>
+      <c r="U23" s="65"/>
+      <c r="V23" s="65"/>
+      <c r="W23" s="65"/>
+      <c r="X23" s="65"/>
+      <c r="Y23" s="65"/>
+      <c r="Z23" s="65"/>
+      <c r="AA23" s="65"/>
+      <c r="AB23" s="62"/>
     </row>
     <row r="24" spans="2:28" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="87" t="s">
+      <c r="B24" s="100" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="81"/>
-      <c r="D24" s="81"/>
-      <c r="E24" s="81"/>
-      <c r="F24" s="81"/>
-      <c r="G24" s="88"/>
-      <c r="H24" s="24" t="s">
+      <c r="C24" s="80"/>
+      <c r="D24" s="80"/>
+      <c r="E24" s="80"/>
+      <c r="F24" s="80"/>
+      <c r="G24" s="101"/>
+      <c r="H24" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="I24" s="23"/>
-      <c r="J24" s="23"/>
-      <c r="K24" s="22"/>
-      <c r="N24" s="61"/>
-      <c r="O24" s="61"/>
-      <c r="P24" s="61"/>
-      <c r="Q24" s="61"/>
-      <c r="R24" s="61"/>
-      <c r="S24" s="61"/>
-      <c r="T24" s="61"/>
-      <c r="U24" s="61"/>
-      <c r="V24" s="61"/>
-      <c r="W24" s="61"/>
-      <c r="X24" s="61"/>
-      <c r="Y24" s="61"/>
-      <c r="Z24" s="61"/>
-      <c r="AA24" s="61"/>
-      <c r="AB24" s="63"/>
+      <c r="I24" s="22"/>
+      <c r="J24" s="22"/>
+      <c r="K24" s="21"/>
+      <c r="N24" s="60"/>
+      <c r="O24" s="60"/>
+      <c r="P24" s="60"/>
+      <c r="Q24" s="60"/>
+      <c r="R24" s="60"/>
+      <c r="S24" s="60"/>
+      <c r="T24" s="60"/>
+      <c r="U24" s="60"/>
+      <c r="V24" s="60"/>
+      <c r="W24" s="60"/>
+      <c r="X24" s="60"/>
+      <c r="Y24" s="60"/>
+      <c r="Z24" s="60"/>
+      <c r="AA24" s="60"/>
+      <c r="AB24" s="62"/>
     </row>
     <row r="25" spans="2:28" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="21" t="s">
+      <c r="B25" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="97"/>
-      <c r="D25" s="97"/>
-      <c r="E25" s="98"/>
-      <c r="F25" s="18" t="s">
+      <c r="C25" s="108"/>
+      <c r="D25" s="108"/>
+      <c r="E25" s="109"/>
+      <c r="F25" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="G25" s="20"/>
-      <c r="H25" s="18" t="s">
+      <c r="G25" s="19"/>
+      <c r="H25" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="I25" s="19"/>
-      <c r="J25" s="18" t="s">
+      <c r="I25" s="18"/>
+      <c r="J25" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="K25" s="17"/>
+      <c r="K25" s="16"/>
       <c r="N25" s="3"/>
-      <c r="AB25" s="63"/>
+      <c r="AB25" s="62"/>
     </row>
     <row r="26" spans="2:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="99" t="s">
+      <c r="B26" s="110" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="100"/>
-      <c r="D26" s="100"/>
-      <c r="E26" s="100"/>
-      <c r="F26" s="100"/>
-      <c r="G26" s="91"/>
-      <c r="H26" s="91"/>
-      <c r="I26" s="91"/>
-      <c r="J26" s="91"/>
-      <c r="K26" s="92"/>
+      <c r="C26" s="111"/>
+      <c r="D26" s="111"/>
+      <c r="E26" s="111"/>
+      <c r="F26" s="111"/>
+      <c r="G26" s="104"/>
+      <c r="H26" s="104"/>
+      <c r="I26" s="104"/>
+      <c r="J26" s="104"/>
+      <c r="K26" s="105"/>
       <c r="N26" s="3"/>
-      <c r="AB26" s="63"/>
+      <c r="AB26" s="62"/>
     </row>
     <row r="27" spans="2:28" ht="2.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="16"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="15"/>
-      <c r="I27" s="15"/>
-      <c r="J27" s="15"/>
-      <c r="K27" s="14"/>
-      <c r="N27" s="62"/>
-      <c r="O27" s="62"/>
-      <c r="P27" s="62"/>
-      <c r="Q27" s="62"/>
-      <c r="R27" s="62"/>
-      <c r="S27" s="62"/>
-      <c r="T27" s="62"/>
-      <c r="U27" s="62"/>
-      <c r="V27" s="62"/>
-      <c r="W27" s="62"/>
-      <c r="X27" s="62"/>
-      <c r="Y27" s="62"/>
-      <c r="Z27" s="62"/>
-      <c r="AA27" s="62"/>
-      <c r="AB27" s="63"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="14"/>
+      <c r="J27" s="14"/>
+      <c r="K27" s="13"/>
+      <c r="N27" s="61"/>
+      <c r="O27" s="61"/>
+      <c r="P27" s="61"/>
+      <c r="Q27" s="61"/>
+      <c r="R27" s="61"/>
+      <c r="S27" s="61"/>
+      <c r="T27" s="61"/>
+      <c r="U27" s="61"/>
+      <c r="V27" s="61"/>
+      <c r="W27" s="61"/>
+      <c r="X27" s="61"/>
+      <c r="Y27" s="61"/>
+      <c r="Z27" s="61"/>
+      <c r="AA27" s="61"/>
+      <c r="AB27" s="62"/>
     </row>
     <row r="28" spans="2:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="89" t="s">
+      <c r="B28" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="C28" s="90"/>
-      <c r="D28" s="90"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
-      <c r="I28" s="13"/>
-      <c r="J28" s="13"/>
-      <c r="K28" s="12"/>
+      <c r="C28" s="103"/>
+      <c r="D28" s="103"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="11"/>
       <c r="N28" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AB28" s="63"/>
+      <c r="AB28" s="62"/>
     </row>
     <row r="29" spans="2:28" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="85" t="s">
+      <c r="B29" s="98" t="s">
         <v>4</v>
       </c>
-      <c r="C29" s="86"/>
-      <c r="D29" s="86"/>
-      <c r="E29" s="86"/>
-      <c r="F29" s="86"/>
-      <c r="G29" s="94"/>
-      <c r="H29" s="11" t="s">
+      <c r="C29" s="99"/>
+      <c r="D29" s="99"/>
+      <c r="E29" s="99"/>
+      <c r="F29" s="99"/>
+      <c r="G29" s="107"/>
+      <c r="H29" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="I29" s="10"/>
-      <c r="J29" s="10"/>
-      <c r="K29" s="9"/>
-      <c r="N29" s="65" t="s">
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="8"/>
+      <c r="N29" s="64" t="s">
         <v>53</v>
       </c>
-      <c r="O29" s="65"/>
-      <c r="P29" s="65"/>
-      <c r="Q29" s="65"/>
-      <c r="R29" s="65"/>
-      <c r="S29" s="65"/>
-      <c r="T29" s="65"/>
-      <c r="X29" s="64" t="s">
+      <c r="O29" s="64"/>
+      <c r="P29" s="64"/>
+      <c r="Q29" s="64"/>
+      <c r="R29" s="64"/>
+      <c r="S29" s="64"/>
+      <c r="T29" s="64"/>
+      <c r="X29" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="Y29" s="64"/>
-      <c r="Z29" s="64"/>
-      <c r="AA29" s="64"/>
-      <c r="AB29" s="63"/>
+      <c r="Y29" s="63"/>
+      <c r="Z29" s="63"/>
+      <c r="AA29" s="63"/>
+      <c r="AB29" s="62"/>
     </row>
     <row r="30" spans="2:28" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C30" s="95"/>
-      <c r="D30" s="95"/>
-      <c r="E30" s="96"/>
-      <c r="F30" s="7" t="s">
+      <c r="C30" s="178"/>
+      <c r="D30" s="178"/>
+      <c r="E30" s="179"/>
+      <c r="F30" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="G30" s="6"/>
+      <c r="G30" s="180"/>
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
       <c r="K30" s="4"/>
-      <c r="AB30" s="63"/>
+      <c r="AB30" s="62"/>
     </row>
     <row r="31" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B31" s="3"/>
-      <c r="N31" s="63"/>
-      <c r="O31" s="63"/>
-      <c r="P31" s="63"/>
-      <c r="Q31" s="63"/>
-      <c r="R31" s="63"/>
-      <c r="S31" s="63"/>
-      <c r="T31" s="63"/>
-      <c r="U31" s="63"/>
-      <c r="V31" s="63"/>
-      <c r="W31" s="63"/>
-      <c r="X31" s="63"/>
-      <c r="Y31" s="63"/>
-      <c r="Z31" s="63"/>
-      <c r="AA31" s="63"/>
-      <c r="AB31" s="63"/>
+      <c r="N31" s="62"/>
+      <c r="O31" s="62"/>
+      <c r="P31" s="62"/>
+      <c r="Q31" s="62"/>
+      <c r="R31" s="62"/>
+      <c r="S31" s="62"/>
+      <c r="T31" s="62"/>
+      <c r="U31" s="62"/>
+      <c r="V31" s="62"/>
+      <c r="W31" s="62"/>
+      <c r="X31" s="62"/>
+      <c r="Y31" s="62"/>
+      <c r="Z31" s="62"/>
+      <c r="AA31" s="62"/>
+      <c r="AB31" s="62"/>
     </row>
     <row r="32" spans="2:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="53"/>
-      <c r="C32" s="53"/>
-      <c r="D32" s="53"/>
-      <c r="E32" s="53"/>
-      <c r="F32" s="53"/>
-      <c r="G32" s="53"/>
-      <c r="H32" s="53"/>
-      <c r="I32" s="53"/>
-      <c r="J32" s="53"/>
-      <c r="K32" s="53"/>
+      <c r="B32" s="52"/>
+      <c r="C32" s="52"/>
+      <c r="D32" s="52"/>
+      <c r="E32" s="52"/>
+      <c r="F32" s="52"/>
+      <c r="G32" s="52"/>
+      <c r="H32" s="52"/>
+      <c r="I32" s="52"/>
+      <c r="J32" s="52"/>
+      <c r="K32" s="52"/>
     </row>
     <row r="33" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B33" s="2" t="s">

</xml_diff>

<commit_message>
Revert "Merge branch 'equipos' of https://github.com/AdonayXX/Frontend into equipos"
This reverts commit b6ab5dd3741ac1dcaaa0d41fd9d28773acaf537c, reversing
changes made to 1883b451b7e81b7ee562dba39deb4d0b0c2202d2.
</commit_message>
<xml_diff>
--- a/documents/ReporteVale.xlsx
+++ b/documents/ReporteVale.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David Duarte Garcia\OneDrive - Universidad Técnica Nacional\Escritorio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4874BF8-2615-4E24-854E-9234BF605845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{301C120F-E069-44AD-BE91-0475B5B13018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{C8E842AF-28D0-4143-9950-C0C2C392F242}"/>
   </bookViews>
@@ -241,7 +241,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\-mm\-yy"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="MS Sans Serif"/>
@@ -379,10 +379,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <name val="MS Sans Serif"/>
-    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1134,6 +1130,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1374,48 +1374,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1448,6 +1406,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="14" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
@@ -1515,6 +1481,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1569,6 +1577,32 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -1614,32 +1648,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
     </xf>
@@ -1678,18 +1686,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous" vertical="top"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2027,8 +2023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{505F8341-330E-4B75-B029-434DF2C2CA09}">
   <dimension ref="B1:AT113"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="AA47" sqref="AA47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2038,10 +2034,10 @@
     <col min="3" max="3" width="4.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="4" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" style="1" customWidth="1"/>
     <col min="7" max="7" width="18.42578125" style="1" customWidth="1"/>
     <col min="8" max="8" width="10.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="2" style="1" customWidth="1"/>
     <col min="10" max="10" width="9.5703125" style="1" customWidth="1"/>
     <col min="11" max="11" width="16.85546875" style="1" customWidth="1"/>
     <col min="12" max="12" width="3.28515625" style="1" hidden="1" customWidth="1"/>
@@ -3767,926 +3763,926 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="165" t="s">
+      <c r="B1" s="168" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="165"/>
-      <c r="D1" s="165"/>
-      <c r="E1" s="165"/>
-      <c r="F1" s="165"/>
-      <c r="G1" s="165"/>
-      <c r="H1" s="165"/>
-      <c r="I1" s="165"/>
-      <c r="J1" s="165"/>
-      <c r="K1" s="165"/>
-      <c r="N1" s="166" t="s">
+      <c r="C1" s="168"/>
+      <c r="D1" s="168"/>
+      <c r="E1" s="168"/>
+      <c r="F1" s="168"/>
+      <c r="G1" s="168"/>
+      <c r="H1" s="168"/>
+      <c r="I1" s="168"/>
+      <c r="J1" s="168"/>
+      <c r="K1" s="168"/>
+      <c r="N1" s="169" t="s">
         <v>33</v>
       </c>
-      <c r="O1" s="166"/>
-      <c r="P1" s="166"/>
-      <c r="Q1" s="166"/>
-      <c r="R1" s="166"/>
-      <c r="S1" s="166"/>
-      <c r="T1" s="166"/>
-      <c r="U1" s="166"/>
-      <c r="V1" s="166"/>
-      <c r="W1" s="166"/>
-      <c r="X1" s="166"/>
-      <c r="Y1" s="166"/>
-      <c r="Z1" s="166"/>
-      <c r="AA1" s="166"/>
-      <c r="AB1" s="62"/>
+      <c r="O1" s="169"/>
+      <c r="P1" s="169"/>
+      <c r="Q1" s="169"/>
+      <c r="R1" s="169"/>
+      <c r="S1" s="169"/>
+      <c r="T1" s="169"/>
+      <c r="U1" s="169"/>
+      <c r="V1" s="169"/>
+      <c r="W1" s="169"/>
+      <c r="X1" s="169"/>
+      <c r="Y1" s="169"/>
+      <c r="Z1" s="169"/>
+      <c r="AA1" s="169"/>
+      <c r="AB1" s="63"/>
     </row>
     <row r="2" spans="2:28" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="167" t="s">
+      <c r="B2" s="170" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="167"/>
-      <c r="D2" s="167"/>
-      <c r="E2" s="167"/>
-      <c r="F2" s="167"/>
-      <c r="G2" s="167"/>
-      <c r="H2" s="167"/>
-      <c r="I2" s="167"/>
-      <c r="J2" s="167"/>
+      <c r="C2" s="170"/>
+      <c r="D2" s="170"/>
+      <c r="E2" s="170"/>
+      <c r="F2" s="170"/>
+      <c r="G2" s="170"/>
+      <c r="H2" s="170"/>
+      <c r="I2" s="170"/>
+      <c r="J2" s="170"/>
       <c r="N2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AB2" s="62"/>
+      <c r="AB2" s="63"/>
     </row>
     <row r="3" spans="2:28" ht="12.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="168" t="s">
+      <c r="B3" s="171" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="168"/>
-      <c r="D3" s="168"/>
-      <c r="E3" s="168"/>
-      <c r="F3" s="168"/>
-      <c r="G3" s="168"/>
-      <c r="H3" s="168"/>
-      <c r="I3" s="168"/>
-      <c r="J3" s="168"/>
-      <c r="N3" s="169" t="s">
+      <c r="C3" s="171"/>
+      <c r="D3" s="171"/>
+      <c r="E3" s="171"/>
+      <c r="F3" s="171"/>
+      <c r="G3" s="171"/>
+      <c r="H3" s="171"/>
+      <c r="I3" s="171"/>
+      <c r="J3" s="171"/>
+      <c r="N3" s="172" t="s">
         <v>34</v>
       </c>
-      <c r="O3" s="170"/>
-      <c r="P3" s="171"/>
-      <c r="Q3" s="171"/>
-      <c r="R3" s="171"/>
-      <c r="S3" s="171"/>
-      <c r="T3" s="171"/>
-      <c r="U3" s="171"/>
-      <c r="V3" s="172"/>
-      <c r="W3" s="173" t="s">
+      <c r="O3" s="173"/>
+      <c r="P3" s="174"/>
+      <c r="Q3" s="174"/>
+      <c r="R3" s="174"/>
+      <c r="S3" s="174"/>
+      <c r="T3" s="174"/>
+      <c r="U3" s="174"/>
+      <c r="V3" s="175"/>
+      <c r="W3" s="176" t="s">
         <v>35</v>
       </c>
-      <c r="X3" s="171"/>
-      <c r="Y3" s="171"/>
-      <c r="Z3" s="171"/>
-      <c r="AA3" s="174"/>
-      <c r="AB3" s="62"/>
+      <c r="X3" s="174"/>
+      <c r="Y3" s="174"/>
+      <c r="Z3" s="174"/>
+      <c r="AA3" s="177"/>
+      <c r="AB3" s="63"/>
     </row>
     <row r="4" spans="2:28" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="167" t="s">
+      <c r="B4" s="170" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="167"/>
-      <c r="D4" s="167"/>
-      <c r="E4" s="167"/>
-      <c r="F4" s="167"/>
-      <c r="G4" s="167"/>
-      <c r="H4" s="167"/>
-      <c r="I4" s="167"/>
-      <c r="J4" s="167"/>
-      <c r="N4" s="53" t="s">
+      <c r="C4" s="170"/>
+      <c r="D4" s="170"/>
+      <c r="E4" s="170"/>
+      <c r="F4" s="170"/>
+      <c r="G4" s="170"/>
+      <c r="H4" s="170"/>
+      <c r="I4" s="170"/>
+      <c r="J4" s="170"/>
+      <c r="N4" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="O4" s="54"/>
-      <c r="P4" s="175" t="s">
+      <c r="O4" s="55"/>
+      <c r="P4" s="178" t="s">
         <v>36</v>
       </c>
-      <c r="Q4" s="175"/>
-      <c r="R4" s="175"/>
-      <c r="S4" s="175"/>
-      <c r="T4" s="175"/>
-      <c r="U4" s="175"/>
-      <c r="V4" s="176"/>
-      <c r="W4" s="55" t="s">
+      <c r="Q4" s="178"/>
+      <c r="R4" s="178"/>
+      <c r="S4" s="178"/>
+      <c r="T4" s="178"/>
+      <c r="U4" s="178"/>
+      <c r="V4" s="179"/>
+      <c r="W4" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="X4" s="56"/>
-      <c r="Y4" s="177" t="s">
+      <c r="X4" s="57"/>
+      <c r="Y4" s="180" t="s">
         <v>37</v>
       </c>
-      <c r="Z4" s="175"/>
-      <c r="AA4" s="57"/>
-      <c r="AB4" s="62"/>
+      <c r="Z4" s="178"/>
+      <c r="AA4" s="58"/>
+      <c r="AB4" s="63"/>
     </row>
     <row r="5" spans="2:28" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="148" t="s">
+      <c r="B5" s="159" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="149"/>
-      <c r="D5" s="149"/>
-      <c r="E5" s="149"/>
-      <c r="F5" s="149"/>
-      <c r="G5" s="149"/>
-      <c r="H5" s="149"/>
-      <c r="I5" s="150"/>
-      <c r="J5" s="47" t="s">
+      <c r="C5" s="160"/>
+      <c r="D5" s="160"/>
+      <c r="E5" s="160"/>
+      <c r="F5" s="160"/>
+      <c r="G5" s="160"/>
+      <c r="H5" s="160"/>
+      <c r="I5" s="161"/>
+      <c r="J5" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="K5" s="46"/>
-      <c r="N5" s="58" t="s">
+      <c r="K5" s="47"/>
+      <c r="N5" s="59" t="s">
         <v>38</v>
       </c>
-      <c r="O5" s="59" t="s">
+      <c r="O5" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="P5" s="131" t="s">
+      <c r="P5" s="134" t="s">
         <v>39</v>
       </c>
-      <c r="Q5" s="151"/>
-      <c r="R5" s="151"/>
-      <c r="S5" s="151"/>
-      <c r="T5" s="151"/>
-      <c r="U5" s="151"/>
-      <c r="V5" s="132"/>
-      <c r="W5" s="131" t="s">
+      <c r="Q5" s="162"/>
+      <c r="R5" s="162"/>
+      <c r="S5" s="162"/>
+      <c r="T5" s="162"/>
+      <c r="U5" s="162"/>
+      <c r="V5" s="135"/>
+      <c r="W5" s="134" t="s">
         <v>40</v>
       </c>
-      <c r="X5" s="151"/>
-      <c r="Y5" s="151"/>
-      <c r="Z5" s="151"/>
-      <c r="AA5" s="152"/>
-      <c r="AB5" s="62"/>
+      <c r="X5" s="162"/>
+      <c r="Y5" s="162"/>
+      <c r="Z5" s="162"/>
+      <c r="AA5" s="163"/>
+      <c r="AB5" s="63"/>
     </row>
     <row r="6" spans="2:28" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="45" t="s">
+      <c r="B6" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="44"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="44"/>
-      <c r="J6" s="44"/>
-      <c r="K6" s="43"/>
-      <c r="N6" s="82" t="s">
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="45"/>
+      <c r="I6" s="45"/>
+      <c r="J6" s="45"/>
+      <c r="K6" s="44"/>
+      <c r="N6" s="83" t="s">
         <v>41</v>
       </c>
-      <c r="O6" s="69"/>
-      <c r="P6" s="71" t="s">
+      <c r="O6" s="70"/>
+      <c r="P6" s="72" t="s">
         <v>42</v>
       </c>
-      <c r="Q6" s="73"/>
-      <c r="R6" s="73"/>
-      <c r="S6" s="75" t="s">
+      <c r="Q6" s="74"/>
+      <c r="R6" s="74"/>
+      <c r="S6" s="76" t="s">
         <v>43</v>
       </c>
-      <c r="T6" s="73"/>
-      <c r="U6" s="77"/>
-      <c r="V6" s="79"/>
-      <c r="W6" s="80"/>
-      <c r="X6" s="80"/>
-      <c r="Y6" s="80"/>
-      <c r="Z6" s="80"/>
-      <c r="AA6" s="81"/>
-      <c r="AB6" s="62"/>
+      <c r="T6" s="74"/>
+      <c r="U6" s="78"/>
+      <c r="V6" s="80"/>
+      <c r="W6" s="81"/>
+      <c r="X6" s="81"/>
+      <c r="Y6" s="81"/>
+      <c r="Z6" s="81"/>
+      <c r="AA6" s="82"/>
+      <c r="AB6" s="63"/>
     </row>
     <row r="7" spans="2:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="157" t="s">
+      <c r="B7" s="147" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="158"/>
-      <c r="D7" s="159" t="s">
+      <c r="C7" s="148"/>
+      <c r="D7" s="149" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="160"/>
-      <c r="F7" s="163"/>
-      <c r="G7" s="163"/>
-      <c r="H7" s="163"/>
-      <c r="I7" s="163"/>
-      <c r="J7" s="163"/>
-      <c r="K7" s="42" t="s">
+      <c r="E7" s="150"/>
+      <c r="F7" s="153"/>
+      <c r="G7" s="153"/>
+      <c r="H7" s="153"/>
+      <c r="I7" s="153"/>
+      <c r="J7" s="153"/>
+      <c r="K7" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="N7" s="83"/>
-      <c r="O7" s="70"/>
-      <c r="P7" s="72"/>
-      <c r="Q7" s="74"/>
-      <c r="R7" s="74"/>
-      <c r="S7" s="76"/>
-      <c r="T7" s="74"/>
-      <c r="U7" s="78"/>
-      <c r="V7" s="79"/>
-      <c r="W7" s="80"/>
-      <c r="X7" s="80"/>
-      <c r="Y7" s="80"/>
-      <c r="Z7" s="80"/>
-      <c r="AA7" s="81"/>
-      <c r="AB7" s="62"/>
+      <c r="N7" s="84"/>
+      <c r="O7" s="71"/>
+      <c r="P7" s="73"/>
+      <c r="Q7" s="75"/>
+      <c r="R7" s="75"/>
+      <c r="S7" s="77"/>
+      <c r="T7" s="75"/>
+      <c r="U7" s="79"/>
+      <c r="V7" s="80"/>
+      <c r="W7" s="81"/>
+      <c r="X7" s="81"/>
+      <c r="Y7" s="81"/>
+      <c r="Z7" s="81"/>
+      <c r="AA7" s="82"/>
+      <c r="AB7" s="63"/>
     </row>
     <row r="8" spans="2:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="144"/>
-      <c r="C8" s="145"/>
-      <c r="D8" s="161"/>
-      <c r="E8" s="162"/>
-      <c r="F8" s="164"/>
-      <c r="G8" s="164"/>
-      <c r="H8" s="164"/>
-      <c r="I8" s="164"/>
-      <c r="J8" s="164"/>
-      <c r="K8" s="41"/>
-      <c r="N8" s="82" t="s">
+      <c r="B8" s="155"/>
+      <c r="C8" s="156"/>
+      <c r="D8" s="151"/>
+      <c r="E8" s="152"/>
+      <c r="F8" s="154"/>
+      <c r="G8" s="154"/>
+      <c r="H8" s="154"/>
+      <c r="I8" s="154"/>
+      <c r="J8" s="154"/>
+      <c r="K8" s="42"/>
+      <c r="N8" s="83" t="s">
         <v>44</v>
       </c>
-      <c r="O8" s="69"/>
-      <c r="P8" s="71" t="s">
+      <c r="O8" s="70"/>
+      <c r="P8" s="72" t="s">
         <v>42</v>
       </c>
-      <c r="Q8" s="73"/>
-      <c r="R8" s="73"/>
-      <c r="S8" s="75" t="s">
+      <c r="Q8" s="74"/>
+      <c r="R8" s="74"/>
+      <c r="S8" s="76" t="s">
         <v>43</v>
       </c>
-      <c r="T8" s="73"/>
-      <c r="U8" s="77"/>
-      <c r="V8" s="79"/>
-      <c r="W8" s="80"/>
-      <c r="X8" s="80"/>
-      <c r="Y8" s="80"/>
-      <c r="Z8" s="80"/>
-      <c r="AA8" s="81"/>
-      <c r="AB8" s="62"/>
+      <c r="T8" s="74"/>
+      <c r="U8" s="78"/>
+      <c r="V8" s="80"/>
+      <c r="W8" s="81"/>
+      <c r="X8" s="81"/>
+      <c r="Y8" s="81"/>
+      <c r="Z8" s="81"/>
+      <c r="AA8" s="82"/>
+      <c r="AB8" s="63"/>
     </row>
     <row r="9" spans="2:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="153"/>
-      <c r="D9" s="153"/>
-      <c r="E9" s="153"/>
-      <c r="F9" s="153"/>
-      <c r="G9" s="153"/>
-      <c r="H9" s="153"/>
-      <c r="I9" s="153"/>
-      <c r="J9" s="153"/>
-      <c r="K9" s="154"/>
-      <c r="N9" s="83"/>
-      <c r="O9" s="70"/>
-      <c r="P9" s="72"/>
-      <c r="Q9" s="74"/>
-      <c r="R9" s="74"/>
-      <c r="S9" s="76"/>
-      <c r="T9" s="74"/>
-      <c r="U9" s="78"/>
-      <c r="V9" s="79"/>
-      <c r="W9" s="80"/>
-      <c r="X9" s="80"/>
-      <c r="Y9" s="80"/>
-      <c r="Z9" s="80"/>
-      <c r="AA9" s="81"/>
-      <c r="AB9" s="62"/>
+      <c r="C9" s="164"/>
+      <c r="D9" s="164"/>
+      <c r="E9" s="164"/>
+      <c r="F9" s="164"/>
+      <c r="G9" s="164"/>
+      <c r="H9" s="164"/>
+      <c r="I9" s="164"/>
+      <c r="J9" s="164"/>
+      <c r="K9" s="165"/>
+      <c r="N9" s="84"/>
+      <c r="O9" s="71"/>
+      <c r="P9" s="73"/>
+      <c r="Q9" s="75"/>
+      <c r="R9" s="75"/>
+      <c r="S9" s="77"/>
+      <c r="T9" s="75"/>
+      <c r="U9" s="79"/>
+      <c r="V9" s="80"/>
+      <c r="W9" s="81"/>
+      <c r="X9" s="81"/>
+      <c r="Y9" s="81"/>
+      <c r="Z9" s="81"/>
+      <c r="AA9" s="82"/>
+      <c r="AB9" s="63"/>
     </row>
     <row r="10" spans="2:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="39"/>
-      <c r="C10" s="142"/>
-      <c r="D10" s="142"/>
-      <c r="E10" s="142"/>
-      <c r="F10" s="142"/>
-      <c r="G10" s="142"/>
-      <c r="H10" s="142"/>
-      <c r="I10" s="142"/>
-      <c r="J10" s="142"/>
-      <c r="K10" s="155"/>
-      <c r="N10" s="82" t="s">
+      <c r="B10" s="40"/>
+      <c r="C10" s="145"/>
+      <c r="D10" s="145"/>
+      <c r="E10" s="145"/>
+      <c r="F10" s="145"/>
+      <c r="G10" s="145"/>
+      <c r="H10" s="145"/>
+      <c r="I10" s="145"/>
+      <c r="J10" s="145"/>
+      <c r="K10" s="166"/>
+      <c r="N10" s="83" t="s">
         <v>45</v>
       </c>
-      <c r="O10" s="69"/>
-      <c r="P10" s="71" t="s">
+      <c r="O10" s="70"/>
+      <c r="P10" s="72" t="s">
         <v>42</v>
       </c>
-      <c r="Q10" s="73"/>
-      <c r="R10" s="73"/>
-      <c r="S10" s="73" t="s">
+      <c r="Q10" s="74"/>
+      <c r="R10" s="74"/>
+      <c r="S10" s="74" t="s">
         <v>43</v>
       </c>
-      <c r="T10" s="73"/>
-      <c r="U10" s="77"/>
-      <c r="V10" s="79"/>
-      <c r="W10" s="80"/>
-      <c r="X10" s="80"/>
-      <c r="Y10" s="80"/>
-      <c r="Z10" s="80"/>
-      <c r="AA10" s="81"/>
-      <c r="AB10" s="62"/>
+      <c r="T10" s="74"/>
+      <c r="U10" s="78"/>
+      <c r="V10" s="80"/>
+      <c r="W10" s="81"/>
+      <c r="X10" s="81"/>
+      <c r="Y10" s="81"/>
+      <c r="Z10" s="81"/>
+      <c r="AA10" s="82"/>
+      <c r="AB10" s="63"/>
     </row>
     <row r="11" spans="2:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="38"/>
-      <c r="C11" s="156"/>
-      <c r="D11" s="156"/>
-      <c r="E11" s="156"/>
-      <c r="F11" s="156"/>
-      <c r="G11" s="156"/>
-      <c r="H11" s="156"/>
-      <c r="I11" s="142"/>
-      <c r="J11" s="142"/>
-      <c r="K11" s="155"/>
-      <c r="N11" s="83"/>
-      <c r="O11" s="70"/>
-      <c r="P11" s="72"/>
-      <c r="Q11" s="74"/>
-      <c r="R11" s="74"/>
-      <c r="S11" s="74"/>
-      <c r="T11" s="74"/>
-      <c r="U11" s="78"/>
-      <c r="V11" s="79"/>
-      <c r="W11" s="80"/>
-      <c r="X11" s="80"/>
-      <c r="Y11" s="80"/>
-      <c r="Z11" s="80"/>
-      <c r="AA11" s="81"/>
-      <c r="AB11" s="62"/>
+      <c r="B11" s="39"/>
+      <c r="C11" s="167"/>
+      <c r="D11" s="167"/>
+      <c r="E11" s="167"/>
+      <c r="F11" s="167"/>
+      <c r="G11" s="167"/>
+      <c r="H11" s="167"/>
+      <c r="I11" s="145"/>
+      <c r="J11" s="145"/>
+      <c r="K11" s="166"/>
+      <c r="N11" s="84"/>
+      <c r="O11" s="71"/>
+      <c r="P11" s="73"/>
+      <c r="Q11" s="75"/>
+      <c r="R11" s="75"/>
+      <c r="S11" s="75"/>
+      <c r="T11" s="75"/>
+      <c r="U11" s="79"/>
+      <c r="V11" s="80"/>
+      <c r="W11" s="81"/>
+      <c r="X11" s="81"/>
+      <c r="Y11" s="81"/>
+      <c r="Z11" s="81"/>
+      <c r="AA11" s="82"/>
+      <c r="AB11" s="63"/>
     </row>
     <row r="12" spans="2:28" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="146" t="s">
+      <c r="B12" s="157" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="147"/>
-      <c r="D12" s="147"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="36" t="s">
+      <c r="C12" s="158"/>
+      <c r="D12" s="158"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="I12" s="138"/>
-      <c r="J12" s="139"/>
-      <c r="K12" s="140"/>
-      <c r="N12" s="82" t="s">
+      <c r="I12" s="141"/>
+      <c r="J12" s="142"/>
+      <c r="K12" s="143"/>
+      <c r="N12" s="83" t="s">
         <v>46</v>
       </c>
-      <c r="O12" s="69"/>
-      <c r="P12" s="71" t="s">
+      <c r="O12" s="70"/>
+      <c r="P12" s="72" t="s">
         <v>42</v>
       </c>
-      <c r="Q12" s="73"/>
-      <c r="R12" s="73"/>
-      <c r="S12" s="75" t="s">
+      <c r="Q12" s="74"/>
+      <c r="R12" s="74"/>
+      <c r="S12" s="76" t="s">
         <v>43</v>
       </c>
-      <c r="T12" s="73"/>
-      <c r="U12" s="77"/>
-      <c r="V12" s="79"/>
-      <c r="W12" s="80"/>
-      <c r="X12" s="80"/>
-      <c r="Y12" s="80"/>
-      <c r="Z12" s="80"/>
-      <c r="AA12" s="81"/>
-      <c r="AB12" s="62"/>
+      <c r="T12" s="74"/>
+      <c r="U12" s="78"/>
+      <c r="V12" s="80"/>
+      <c r="W12" s="81"/>
+      <c r="X12" s="81"/>
+      <c r="Y12" s="81"/>
+      <c r="Z12" s="81"/>
+      <c r="AA12" s="82"/>
+      <c r="AB12" s="63"/>
     </row>
     <row r="13" spans="2:28" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="141"/>
-      <c r="C13" s="142"/>
-      <c r="D13" s="142"/>
-      <c r="E13" s="142"/>
-      <c r="F13" s="142"/>
-      <c r="G13" s="142"/>
-      <c r="H13" s="143"/>
-      <c r="I13" s="138"/>
-      <c r="J13" s="139"/>
-      <c r="K13" s="140"/>
-      <c r="N13" s="83"/>
-      <c r="O13" s="70"/>
-      <c r="P13" s="72"/>
-      <c r="Q13" s="74"/>
-      <c r="R13" s="74"/>
-      <c r="S13" s="76"/>
-      <c r="T13" s="74"/>
-      <c r="U13" s="78"/>
-      <c r="V13" s="79"/>
-      <c r="W13" s="80"/>
-      <c r="X13" s="80"/>
-      <c r="Y13" s="80"/>
-      <c r="Z13" s="80"/>
-      <c r="AA13" s="81"/>
-      <c r="AB13" s="62"/>
+      <c r="B13" s="144"/>
+      <c r="C13" s="145"/>
+      <c r="D13" s="145"/>
+      <c r="E13" s="145"/>
+      <c r="F13" s="145"/>
+      <c r="G13" s="145"/>
+      <c r="H13" s="146"/>
+      <c r="I13" s="141"/>
+      <c r="J13" s="142"/>
+      <c r="K13" s="143"/>
+      <c r="N13" s="84"/>
+      <c r="O13" s="71"/>
+      <c r="P13" s="73"/>
+      <c r="Q13" s="75"/>
+      <c r="R13" s="75"/>
+      <c r="S13" s="77"/>
+      <c r="T13" s="75"/>
+      <c r="U13" s="79"/>
+      <c r="V13" s="80"/>
+      <c r="W13" s="81"/>
+      <c r="X13" s="81"/>
+      <c r="Y13" s="81"/>
+      <c r="Z13" s="81"/>
+      <c r="AA13" s="82"/>
+      <c r="AB13" s="63"/>
     </row>
     <row r="14" spans="2:28" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="49"/>
-      <c r="C14" s="50"/>
-      <c r="D14" s="50"/>
-      <c r="E14" s="50"/>
-      <c r="F14" s="50"/>
-      <c r="G14" s="50"/>
-      <c r="H14" s="50"/>
-      <c r="I14" s="138"/>
-      <c r="J14" s="139"/>
-      <c r="K14" s="140"/>
-      <c r="N14" s="67" t="s">
+      <c r="B14" s="50"/>
+      <c r="C14" s="51"/>
+      <c r="D14" s="51"/>
+      <c r="E14" s="51"/>
+      <c r="F14" s="51"/>
+      <c r="G14" s="51"/>
+      <c r="H14" s="51"/>
+      <c r="I14" s="141"/>
+      <c r="J14" s="142"/>
+      <c r="K14" s="143"/>
+      <c r="N14" s="68" t="s">
         <v>47</v>
       </c>
-      <c r="O14" s="69"/>
-      <c r="P14" s="71" t="s">
+      <c r="O14" s="70"/>
+      <c r="P14" s="72" t="s">
         <v>42</v>
       </c>
-      <c r="Q14" s="73"/>
-      <c r="R14" s="73"/>
-      <c r="S14" s="75" t="s">
+      <c r="Q14" s="74"/>
+      <c r="R14" s="74"/>
+      <c r="S14" s="76" t="s">
         <v>43</v>
       </c>
-      <c r="T14" s="73"/>
-      <c r="U14" s="77"/>
-      <c r="V14" s="79"/>
-      <c r="W14" s="80"/>
-      <c r="X14" s="80"/>
-      <c r="Y14" s="80"/>
-      <c r="Z14" s="80"/>
-      <c r="AA14" s="81"/>
-      <c r="AB14" s="62"/>
+      <c r="T14" s="74"/>
+      <c r="U14" s="78"/>
+      <c r="V14" s="80"/>
+      <c r="W14" s="81"/>
+      <c r="X14" s="81"/>
+      <c r="Y14" s="81"/>
+      <c r="Z14" s="81"/>
+      <c r="AA14" s="82"/>
+      <c r="AB14" s="63"/>
     </row>
     <row r="15" spans="2:28" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="49"/>
-      <c r="C15" s="50"/>
-      <c r="D15" s="50"/>
-      <c r="E15" s="50"/>
-      <c r="F15" s="50"/>
-      <c r="G15" s="50"/>
-      <c r="H15" s="50"/>
-      <c r="I15" s="138"/>
-      <c r="J15" s="139"/>
-      <c r="K15" s="140"/>
-      <c r="N15" s="68"/>
-      <c r="O15" s="70"/>
-      <c r="P15" s="72"/>
-      <c r="Q15" s="74"/>
-      <c r="R15" s="74"/>
-      <c r="S15" s="76"/>
-      <c r="T15" s="74"/>
-      <c r="U15" s="78"/>
-      <c r="V15" s="79"/>
-      <c r="W15" s="80"/>
-      <c r="X15" s="80"/>
-      <c r="Y15" s="80"/>
-      <c r="Z15" s="80"/>
-      <c r="AA15" s="81"/>
-      <c r="AB15" s="62"/>
+      <c r="B15" s="50"/>
+      <c r="C15" s="51"/>
+      <c r="D15" s="51"/>
+      <c r="E15" s="51"/>
+      <c r="F15" s="51"/>
+      <c r="G15" s="51"/>
+      <c r="H15" s="51"/>
+      <c r="I15" s="141"/>
+      <c r="J15" s="142"/>
+      <c r="K15" s="143"/>
+      <c r="N15" s="69"/>
+      <c r="O15" s="71"/>
+      <c r="P15" s="73"/>
+      <c r="Q15" s="75"/>
+      <c r="R15" s="75"/>
+      <c r="S15" s="77"/>
+      <c r="T15" s="75"/>
+      <c r="U15" s="79"/>
+      <c r="V15" s="80"/>
+      <c r="W15" s="81"/>
+      <c r="X15" s="81"/>
+      <c r="Y15" s="81"/>
+      <c r="Z15" s="81"/>
+      <c r="AA15" s="82"/>
+      <c r="AB15" s="63"/>
     </row>
     <row r="16" spans="2:28" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="49"/>
-      <c r="C16" s="50"/>
-      <c r="D16" s="50"/>
-      <c r="E16" s="50"/>
-      <c r="F16" s="50"/>
-      <c r="G16" s="50"/>
-      <c r="H16" s="51"/>
-      <c r="I16" s="138"/>
-      <c r="J16" s="139"/>
-      <c r="K16" s="140"/>
-      <c r="N16" s="82" t="s">
+      <c r="B16" s="50"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="51"/>
+      <c r="G16" s="51"/>
+      <c r="H16" s="52"/>
+      <c r="I16" s="141"/>
+      <c r="J16" s="142"/>
+      <c r="K16" s="143"/>
+      <c r="N16" s="83" t="s">
         <v>48</v>
       </c>
-      <c r="O16" s="69"/>
-      <c r="P16" s="71" t="s">
+      <c r="O16" s="70"/>
+      <c r="P16" s="72" t="s">
         <v>42</v>
       </c>
-      <c r="Q16" s="73"/>
-      <c r="R16" s="73"/>
-      <c r="S16" s="75" t="s">
+      <c r="Q16" s="74"/>
+      <c r="R16" s="74"/>
+      <c r="S16" s="76" t="s">
         <v>43</v>
       </c>
-      <c r="T16" s="73"/>
-      <c r="U16" s="77"/>
-      <c r="V16" s="79"/>
-      <c r="W16" s="80"/>
-      <c r="X16" s="80"/>
-      <c r="Y16" s="80"/>
-      <c r="Z16" s="80"/>
-      <c r="AA16" s="81"/>
-      <c r="AB16" s="62"/>
+      <c r="T16" s="74"/>
+      <c r="U16" s="78"/>
+      <c r="V16" s="80"/>
+      <c r="W16" s="81"/>
+      <c r="X16" s="81"/>
+      <c r="Y16" s="81"/>
+      <c r="Z16" s="81"/>
+      <c r="AA16" s="82"/>
+      <c r="AB16" s="63"/>
     </row>
     <row r="17" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="128" t="s">
+      <c r="B17" s="131" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="129"/>
-      <c r="D17" s="129"/>
-      <c r="E17" s="129"/>
-      <c r="F17" s="130"/>
-      <c r="G17" s="133"/>
-      <c r="H17" s="134"/>
-      <c r="I17" s="134"/>
-      <c r="J17" s="134"/>
-      <c r="K17" s="135"/>
-      <c r="N17" s="83"/>
-      <c r="O17" s="70"/>
-      <c r="P17" s="72"/>
-      <c r="Q17" s="74"/>
-      <c r="R17" s="74"/>
-      <c r="S17" s="76"/>
-      <c r="T17" s="74"/>
-      <c r="U17" s="78"/>
-      <c r="V17" s="79"/>
-      <c r="W17" s="80"/>
-      <c r="X17" s="80"/>
-      <c r="Y17" s="80"/>
-      <c r="Z17" s="80"/>
-      <c r="AA17" s="81"/>
-      <c r="AB17" s="62"/>
+      <c r="C17" s="132"/>
+      <c r="D17" s="132"/>
+      <c r="E17" s="132"/>
+      <c r="F17" s="133"/>
+      <c r="G17" s="136"/>
+      <c r="H17" s="137"/>
+      <c r="I17" s="137"/>
+      <c r="J17" s="137"/>
+      <c r="K17" s="138"/>
+      <c r="N17" s="84"/>
+      <c r="O17" s="71"/>
+      <c r="P17" s="73"/>
+      <c r="Q17" s="75"/>
+      <c r="R17" s="75"/>
+      <c r="S17" s="77"/>
+      <c r="T17" s="75"/>
+      <c r="U17" s="79"/>
+      <c r="V17" s="80"/>
+      <c r="W17" s="81"/>
+      <c r="X17" s="81"/>
+      <c r="Y17" s="81"/>
+      <c r="Z17" s="81"/>
+      <c r="AA17" s="82"/>
+      <c r="AB17" s="63"/>
     </row>
     <row r="18" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="35"/>
-      <c r="C18" s="131" t="s">
+      <c r="B18" s="36"/>
+      <c r="C18" s="134" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="132"/>
-      <c r="E18" s="131" t="s">
+      <c r="D18" s="135"/>
+      <c r="E18" s="134" t="s">
         <v>20</v>
       </c>
-      <c r="F18" s="132"/>
-      <c r="G18" s="48" t="s">
+      <c r="F18" s="135"/>
+      <c r="G18" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="H18" s="136"/>
-      <c r="I18" s="136"/>
-      <c r="J18" s="136"/>
-      <c r="K18" s="137"/>
-      <c r="N18" s="122" t="s">
+      <c r="H18" s="139"/>
+      <c r="I18" s="139"/>
+      <c r="J18" s="139"/>
+      <c r="K18" s="140"/>
+      <c r="N18" s="111" t="s">
         <v>49</v>
       </c>
-      <c r="O18" s="125"/>
-      <c r="P18" s="84" t="s">
+      <c r="O18" s="114"/>
+      <c r="P18" s="117" t="s">
         <v>42</v>
       </c>
-      <c r="Q18" s="84"/>
-      <c r="R18" s="84"/>
-      <c r="S18" s="87" t="s">
+      <c r="Q18" s="117"/>
+      <c r="R18" s="117"/>
+      <c r="S18" s="120" t="s">
         <v>43</v>
       </c>
-      <c r="T18" s="73"/>
-      <c r="U18" s="73"/>
-      <c r="V18" s="79"/>
-      <c r="W18" s="80"/>
-      <c r="X18" s="80"/>
-      <c r="Y18" s="80"/>
-      <c r="Z18" s="80"/>
-      <c r="AA18" s="81"/>
-      <c r="AB18" s="62"/>
+      <c r="T18" s="74"/>
+      <c r="U18" s="74"/>
+      <c r="V18" s="80"/>
+      <c r="W18" s="81"/>
+      <c r="X18" s="81"/>
+      <c r="Y18" s="81"/>
+      <c r="Z18" s="81"/>
+      <c r="AA18" s="82"/>
+      <c r="AB18" s="63"/>
     </row>
     <row r="19" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="32" t="s">
+      <c r="B19" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="115"/>
-      <c r="D19" s="116"/>
-      <c r="E19" s="117"/>
-      <c r="F19" s="118"/>
-      <c r="G19" s="34" t="s">
+      <c r="C19" s="104"/>
+      <c r="D19" s="105"/>
+      <c r="E19" s="106"/>
+      <c r="F19" s="107"/>
+      <c r="G19" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="H19" s="33"/>
-      <c r="I19" s="33"/>
-      <c r="J19" s="119"/>
-      <c r="K19" s="120"/>
-      <c r="N19" s="123"/>
-      <c r="O19" s="126"/>
-      <c r="P19" s="85"/>
-      <c r="Q19" s="85"/>
-      <c r="R19" s="85"/>
-      <c r="S19" s="88"/>
-      <c r="T19" s="90"/>
-      <c r="U19" s="90"/>
-      <c r="V19" s="91"/>
-      <c r="W19" s="73"/>
-      <c r="X19" s="73"/>
-      <c r="Y19" s="73"/>
-      <c r="Z19" s="73"/>
-      <c r="AA19" s="92"/>
-      <c r="AB19" s="62"/>
+      <c r="H19" s="34"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="108"/>
+      <c r="K19" s="109"/>
+      <c r="N19" s="112"/>
+      <c r="O19" s="115"/>
+      <c r="P19" s="118"/>
+      <c r="Q19" s="118"/>
+      <c r="R19" s="118"/>
+      <c r="S19" s="121"/>
+      <c r="T19" s="123"/>
+      <c r="U19" s="123"/>
+      <c r="V19" s="124"/>
+      <c r="W19" s="74"/>
+      <c r="X19" s="74"/>
+      <c r="Y19" s="74"/>
+      <c r="Z19" s="74"/>
+      <c r="AA19" s="125"/>
+      <c r="AB19" s="63"/>
     </row>
     <row r="20" spans="2:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="32" t="s">
+      <c r="B20" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="112"/>
-      <c r="D20" s="121"/>
-      <c r="E20" s="112"/>
-      <c r="F20" s="113"/>
-      <c r="G20" s="31"/>
-      <c r="H20" s="30"/>
-      <c r="I20" s="30"/>
-      <c r="J20" s="74" t="s">
+      <c r="C20" s="101"/>
+      <c r="D20" s="110"/>
+      <c r="E20" s="101"/>
+      <c r="F20" s="102"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="31"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="75" t="s">
         <v>16</v>
       </c>
-      <c r="K20" s="114"/>
-      <c r="N20" s="124"/>
-      <c r="O20" s="127"/>
-      <c r="P20" s="86"/>
-      <c r="Q20" s="86"/>
-      <c r="R20" s="86"/>
-      <c r="S20" s="89"/>
-      <c r="T20" s="74"/>
-      <c r="U20" s="74"/>
-      <c r="V20" s="93"/>
-      <c r="W20" s="74"/>
-      <c r="X20" s="74"/>
-      <c r="Y20" s="74"/>
-      <c r="Z20" s="74"/>
-      <c r="AA20" s="94"/>
-      <c r="AB20" s="62"/>
+      <c r="K20" s="103"/>
+      <c r="N20" s="113"/>
+      <c r="O20" s="116"/>
+      <c r="P20" s="119"/>
+      <c r="Q20" s="119"/>
+      <c r="R20" s="119"/>
+      <c r="S20" s="122"/>
+      <c r="T20" s="75"/>
+      <c r="U20" s="75"/>
+      <c r="V20" s="126"/>
+      <c r="W20" s="75"/>
+      <c r="X20" s="75"/>
+      <c r="Y20" s="75"/>
+      <c r="Z20" s="75"/>
+      <c r="AA20" s="127"/>
+      <c r="AB20" s="63"/>
     </row>
     <row r="21" spans="2:28" ht="1.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="20">
+      <c r="B21" s="21">
         <v>2</v>
       </c>
-      <c r="C21" s="29" t="s">
+      <c r="C21" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="29"/>
-      <c r="E21" s="29"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="28"/>
-      <c r="I21" s="28"/>
-      <c r="J21" s="28"/>
-      <c r="K21" s="27"/>
-      <c r="N21" s="95" t="s">
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="29"/>
+      <c r="K21" s="28"/>
+      <c r="N21" s="128" t="s">
         <v>50</v>
       </c>
-      <c r="O21" s="96"/>
-      <c r="P21" s="96"/>
-      <c r="Q21" s="96"/>
-      <c r="R21" s="96"/>
-      <c r="S21" s="96"/>
-      <c r="T21" s="96"/>
-      <c r="U21" s="96"/>
-      <c r="V21" s="96"/>
-      <c r="W21" s="96"/>
-      <c r="X21" s="96"/>
-      <c r="Y21" s="96"/>
-      <c r="Z21" s="96"/>
-      <c r="AA21" s="97"/>
-      <c r="AB21" s="62"/>
+      <c r="O21" s="129"/>
+      <c r="P21" s="129"/>
+      <c r="Q21" s="129"/>
+      <c r="R21" s="129"/>
+      <c r="S21" s="129"/>
+      <c r="T21" s="129"/>
+      <c r="U21" s="129"/>
+      <c r="V21" s="129"/>
+      <c r="W21" s="129"/>
+      <c r="X21" s="129"/>
+      <c r="Y21" s="129"/>
+      <c r="Z21" s="129"/>
+      <c r="AA21" s="130"/>
+      <c r="AB21" s="63"/>
     </row>
     <row r="22" spans="2:28" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="98" t="s">
+      <c r="B22" s="85" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="99"/>
-      <c r="D22" s="99"/>
-      <c r="E22" s="99"/>
-      <c r="F22" s="99"/>
-      <c r="G22" s="99"/>
-      <c r="H22" s="99"/>
-      <c r="I22" s="99"/>
-      <c r="J22" s="99"/>
-      <c r="K22" s="106"/>
-      <c r="N22" s="66" t="s">
+      <c r="C22" s="86"/>
+      <c r="D22" s="86"/>
+      <c r="E22" s="86"/>
+      <c r="F22" s="86"/>
+      <c r="G22" s="86"/>
+      <c r="H22" s="86"/>
+      <c r="I22" s="86"/>
+      <c r="J22" s="86"/>
+      <c r="K22" s="93"/>
+      <c r="N22" s="67" t="s">
         <v>51</v>
       </c>
-      <c r="O22" s="66"/>
-      <c r="P22" s="66"/>
-      <c r="Q22" s="66"/>
-      <c r="R22" s="66"/>
-      <c r="S22" s="66"/>
-      <c r="T22" s="66"/>
-      <c r="U22" s="66"/>
-      <c r="V22" s="66"/>
-      <c r="W22" s="66"/>
-      <c r="X22" s="66"/>
-      <c r="Y22" s="66"/>
-      <c r="Z22" s="66"/>
-      <c r="AA22" s="66"/>
-      <c r="AB22" s="62"/>
+      <c r="O22" s="67"/>
+      <c r="P22" s="67"/>
+      <c r="Q22" s="67"/>
+      <c r="R22" s="67"/>
+      <c r="S22" s="67"/>
+      <c r="T22" s="67"/>
+      <c r="U22" s="67"/>
+      <c r="V22" s="67"/>
+      <c r="W22" s="67"/>
+      <c r="X22" s="67"/>
+      <c r="Y22" s="67"/>
+      <c r="Z22" s="67"/>
+      <c r="AA22" s="67"/>
+      <c r="AB22" s="63"/>
     </row>
     <row r="23" spans="2:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="98" t="s">
+      <c r="B23" s="85" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="99"/>
-      <c r="D23" s="99"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="25"/>
-      <c r="H23" s="26" t="s">
+      <c r="C23" s="86"/>
+      <c r="D23" s="86"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="I23" s="25"/>
-      <c r="J23" s="25"/>
-      <c r="K23" s="24"/>
-      <c r="N23" s="65" t="s">
+      <c r="I23" s="26"/>
+      <c r="J23" s="26"/>
+      <c r="K23" s="25"/>
+      <c r="N23" s="66" t="s">
         <v>52</v>
       </c>
-      <c r="O23" s="65"/>
-      <c r="P23" s="65"/>
-      <c r="Q23" s="65"/>
-      <c r="R23" s="65"/>
-      <c r="S23" s="65"/>
-      <c r="T23" s="65"/>
-      <c r="U23" s="65"/>
-      <c r="V23" s="65"/>
-      <c r="W23" s="65"/>
-      <c r="X23" s="65"/>
-      <c r="Y23" s="65"/>
-      <c r="Z23" s="65"/>
-      <c r="AA23" s="65"/>
-      <c r="AB23" s="62"/>
+      <c r="O23" s="66"/>
+      <c r="P23" s="66"/>
+      <c r="Q23" s="66"/>
+      <c r="R23" s="66"/>
+      <c r="S23" s="66"/>
+      <c r="T23" s="66"/>
+      <c r="U23" s="66"/>
+      <c r="V23" s="66"/>
+      <c r="W23" s="66"/>
+      <c r="X23" s="66"/>
+      <c r="Y23" s="66"/>
+      <c r="Z23" s="66"/>
+      <c r="AA23" s="66"/>
+      <c r="AB23" s="63"/>
     </row>
     <row r="24" spans="2:28" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="100" t="s">
+      <c r="B24" s="87" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="80"/>
-      <c r="D24" s="80"/>
-      <c r="E24" s="80"/>
-      <c r="F24" s="80"/>
-      <c r="G24" s="101"/>
-      <c r="H24" s="23" t="s">
+      <c r="C24" s="81"/>
+      <c r="D24" s="81"/>
+      <c r="E24" s="81"/>
+      <c r="F24" s="81"/>
+      <c r="G24" s="88"/>
+      <c r="H24" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="I24" s="22"/>
-      <c r="J24" s="22"/>
-      <c r="K24" s="21"/>
-      <c r="N24" s="60"/>
-      <c r="O24" s="60"/>
-      <c r="P24" s="60"/>
-      <c r="Q24" s="60"/>
-      <c r="R24" s="60"/>
-      <c r="S24" s="60"/>
-      <c r="T24" s="60"/>
-      <c r="U24" s="60"/>
-      <c r="V24" s="60"/>
-      <c r="W24" s="60"/>
-      <c r="X24" s="60"/>
-      <c r="Y24" s="60"/>
-      <c r="Z24" s="60"/>
-      <c r="AA24" s="60"/>
-      <c r="AB24" s="62"/>
+      <c r="I24" s="23"/>
+      <c r="J24" s="23"/>
+      <c r="K24" s="22"/>
+      <c r="N24" s="61"/>
+      <c r="O24" s="61"/>
+      <c r="P24" s="61"/>
+      <c r="Q24" s="61"/>
+      <c r="R24" s="61"/>
+      <c r="S24" s="61"/>
+      <c r="T24" s="61"/>
+      <c r="U24" s="61"/>
+      <c r="V24" s="61"/>
+      <c r="W24" s="61"/>
+      <c r="X24" s="61"/>
+      <c r="Y24" s="61"/>
+      <c r="Z24" s="61"/>
+      <c r="AA24" s="61"/>
+      <c r="AB24" s="63"/>
     </row>
     <row r="25" spans="2:28" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="20" t="s">
+      <c r="B25" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="108"/>
-      <c r="D25" s="108"/>
-      <c r="E25" s="109"/>
-      <c r="F25" s="17" t="s">
+      <c r="C25" s="97"/>
+      <c r="D25" s="97"/>
+      <c r="E25" s="98"/>
+      <c r="F25" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="G25" s="19"/>
-      <c r="H25" s="17" t="s">
+      <c r="G25" s="20"/>
+      <c r="H25" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="I25" s="18"/>
-      <c r="J25" s="17" t="s">
+      <c r="I25" s="19"/>
+      <c r="J25" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="K25" s="16"/>
+      <c r="K25" s="17"/>
       <c r="N25" s="3"/>
-      <c r="AB25" s="62"/>
+      <c r="AB25" s="63"/>
     </row>
     <row r="26" spans="2:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="110" t="s">
+      <c r="B26" s="99" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="111"/>
-      <c r="D26" s="111"/>
-      <c r="E26" s="111"/>
-      <c r="F26" s="111"/>
-      <c r="G26" s="104"/>
-      <c r="H26" s="104"/>
-      <c r="I26" s="104"/>
-      <c r="J26" s="104"/>
-      <c r="K26" s="105"/>
+      <c r="C26" s="100"/>
+      <c r="D26" s="100"/>
+      <c r="E26" s="100"/>
+      <c r="F26" s="100"/>
+      <c r="G26" s="91"/>
+      <c r="H26" s="91"/>
+      <c r="I26" s="91"/>
+      <c r="J26" s="91"/>
+      <c r="K26" s="92"/>
       <c r="N26" s="3"/>
-      <c r="AB26" s="62"/>
+      <c r="AB26" s="63"/>
     </row>
     <row r="27" spans="2:28" ht="2.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="15"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="14"/>
-      <c r="J27" s="14"/>
-      <c r="K27" s="13"/>
-      <c r="N27" s="61"/>
-      <c r="O27" s="61"/>
-      <c r="P27" s="61"/>
-      <c r="Q27" s="61"/>
-      <c r="R27" s="61"/>
-      <c r="S27" s="61"/>
-      <c r="T27" s="61"/>
-      <c r="U27" s="61"/>
-      <c r="V27" s="61"/>
-      <c r="W27" s="61"/>
-      <c r="X27" s="61"/>
-      <c r="Y27" s="61"/>
-      <c r="Z27" s="61"/>
-      <c r="AA27" s="61"/>
-      <c r="AB27" s="62"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="15"/>
+      <c r="J27" s="15"/>
+      <c r="K27" s="14"/>
+      <c r="N27" s="62"/>
+      <c r="O27" s="62"/>
+      <c r="P27" s="62"/>
+      <c r="Q27" s="62"/>
+      <c r="R27" s="62"/>
+      <c r="S27" s="62"/>
+      <c r="T27" s="62"/>
+      <c r="U27" s="62"/>
+      <c r="V27" s="62"/>
+      <c r="W27" s="62"/>
+      <c r="X27" s="62"/>
+      <c r="Y27" s="62"/>
+      <c r="Z27" s="62"/>
+      <c r="AA27" s="62"/>
+      <c r="AB27" s="63"/>
     </row>
     <row r="28" spans="2:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="102" t="s">
+      <c r="B28" s="89" t="s">
         <v>5</v>
       </c>
-      <c r="C28" s="103"/>
-      <c r="D28" s="103"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
-      <c r="I28" s="12"/>
-      <c r="J28" s="12"/>
-      <c r="K28" s="11"/>
+      <c r="C28" s="90"/>
+      <c r="D28" s="90"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="12"/>
       <c r="N28" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AB28" s="62"/>
+      <c r="AB28" s="63"/>
     </row>
     <row r="29" spans="2:28" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="98" t="s">
+      <c r="B29" s="85" t="s">
         <v>4</v>
       </c>
-      <c r="C29" s="99"/>
-      <c r="D29" s="99"/>
-      <c r="E29" s="99"/>
-      <c r="F29" s="99"/>
-      <c r="G29" s="107"/>
-      <c r="H29" s="10" t="s">
+      <c r="C29" s="86"/>
+      <c r="D29" s="86"/>
+      <c r="E29" s="86"/>
+      <c r="F29" s="86"/>
+      <c r="G29" s="94"/>
+      <c r="H29" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="I29" s="9"/>
-      <c r="J29" s="9"/>
-      <c r="K29" s="8"/>
-      <c r="N29" s="64" t="s">
+      <c r="I29" s="10"/>
+      <c r="J29" s="10"/>
+      <c r="K29" s="9"/>
+      <c r="N29" s="65" t="s">
         <v>53</v>
       </c>
-      <c r="O29" s="64"/>
-      <c r="P29" s="64"/>
-      <c r="Q29" s="64"/>
-      <c r="R29" s="64"/>
-      <c r="S29" s="64"/>
-      <c r="T29" s="64"/>
-      <c r="X29" s="63" t="s">
+      <c r="O29" s="65"/>
+      <c r="P29" s="65"/>
+      <c r="Q29" s="65"/>
+      <c r="R29" s="65"/>
+      <c r="S29" s="65"/>
+      <c r="T29" s="65"/>
+      <c r="X29" s="64" t="s">
         <v>54</v>
       </c>
-      <c r="Y29" s="63"/>
-      <c r="Z29" s="63"/>
-      <c r="AA29" s="63"/>
-      <c r="AB29" s="62"/>
+      <c r="Y29" s="64"/>
+      <c r="Z29" s="64"/>
+      <c r="AA29" s="64"/>
+      <c r="AB29" s="63"/>
     </row>
     <row r="30" spans="2:28" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="7" t="s">
+      <c r="B30" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C30" s="178"/>
-      <c r="D30" s="178"/>
-      <c r="E30" s="179"/>
-      <c r="F30" s="6" t="s">
+      <c r="C30" s="95"/>
+      <c r="D30" s="95"/>
+      <c r="E30" s="96"/>
+      <c r="F30" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="G30" s="180"/>
+      <c r="G30" s="6"/>
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
       <c r="K30" s="4"/>
-      <c r="AB30" s="62"/>
+      <c r="AB30" s="63"/>
     </row>
     <row r="31" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B31" s="3"/>
-      <c r="N31" s="62"/>
-      <c r="O31" s="62"/>
-      <c r="P31" s="62"/>
-      <c r="Q31" s="62"/>
-      <c r="R31" s="62"/>
-      <c r="S31" s="62"/>
-      <c r="T31" s="62"/>
-      <c r="U31" s="62"/>
-      <c r="V31" s="62"/>
-      <c r="W31" s="62"/>
-      <c r="X31" s="62"/>
-      <c r="Y31" s="62"/>
-      <c r="Z31" s="62"/>
-      <c r="AA31" s="62"/>
-      <c r="AB31" s="62"/>
+      <c r="N31" s="63"/>
+      <c r="O31" s="63"/>
+      <c r="P31" s="63"/>
+      <c r="Q31" s="63"/>
+      <c r="R31" s="63"/>
+      <c r="S31" s="63"/>
+      <c r="T31" s="63"/>
+      <c r="U31" s="63"/>
+      <c r="V31" s="63"/>
+      <c r="W31" s="63"/>
+      <c r="X31" s="63"/>
+      <c r="Y31" s="63"/>
+      <c r="Z31" s="63"/>
+      <c r="AA31" s="63"/>
+      <c r="AB31" s="63"/>
     </row>
     <row r="32" spans="2:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="52"/>
-      <c r="C32" s="52"/>
-      <c r="D32" s="52"/>
-      <c r="E32" s="52"/>
-      <c r="F32" s="52"/>
-      <c r="G32" s="52"/>
-      <c r="H32" s="52"/>
-      <c r="I32" s="52"/>
-      <c r="J32" s="52"/>
-      <c r="K32" s="52"/>
+      <c r="B32" s="53"/>
+      <c r="C32" s="53"/>
+      <c r="D32" s="53"/>
+      <c r="E32" s="53"/>
+      <c r="F32" s="53"/>
+      <c r="G32" s="53"/>
+      <c r="H32" s="53"/>
+      <c r="I32" s="53"/>
+      <c r="J32" s="53"/>
+      <c r="K32" s="53"/>
     </row>
     <row r="33" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B33" s="2" t="s">

</xml_diff>